<commit_message>
after labs and lection 29.04.17
</commit_message>
<xml_diff>
--- a/весна/ТМОГИ.2017.весна.xlsx
+++ b/весна/ТМОГИ.2017.весна.xlsx
@@ -1504,7 +1504,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="256">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2053,14 +2053,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2102,7 +2099,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2187,13 +2193,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2611,10 +2610,10 @@
   <dimension ref="A1:CH125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY11" sqref="AY11"/>
+      <selection pane="bottomRight" activeCell="BO18" sqref="BO18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -2652,32 +2651,32 @@
     <col min="50" max="79" width="3.28515625" style="2" customWidth="1"/>
     <col min="80" max="80" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="81" max="82" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="83" max="86" width="0" style="2" hidden="1"/>
+    <col min="83" max="86" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="87" max="16384" width="9.140625" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:82" s="136" customFormat="1" ht="21">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="212" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="213"/>
-      <c r="C1" s="213"/>
-      <c r="D1" s="213"/>
-      <c r="E1" s="214" t="s">
+      <c r="B1" s="212"/>
+      <c r="C1" s="212"/>
+      <c r="D1" s="212"/>
+      <c r="E1" s="213" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="214"/>
-      <c r="G1" s="214"/>
-      <c r="H1" s="214"/>
-      <c r="I1" s="214"/>
-      <c r="J1" s="214"/>
-      <c r="K1" s="214"/>
-      <c r="L1" s="214"/>
-      <c r="M1" s="214"/>
-      <c r="N1" s="214"/>
-      <c r="O1" s="214"/>
-      <c r="P1" s="214"/>
-      <c r="Q1" s="214"/>
+      <c r="F1" s="213"/>
+      <c r="G1" s="213"/>
+      <c r="H1" s="213"/>
+      <c r="I1" s="213"/>
+      <c r="J1" s="213"/>
+      <c r="K1" s="213"/>
+      <c r="L1" s="213"/>
+      <c r="M1" s="213"/>
+      <c r="N1" s="213"/>
+      <c r="O1" s="213"/>
+      <c r="P1" s="213"/>
+      <c r="Q1" s="213"/>
       <c r="R1" s="135"/>
       <c r="S1" s="135"/>
       <c r="T1" s="135"/>
@@ -2700,69 +2699,69 @@
       </c>
       <c r="E2" s="130"/>
       <c r="F2" s="130"/>
-      <c r="G2" s="210" t="s">
+      <c r="G2" s="223" t="s">
         <v>117</v>
       </c>
-      <c r="H2" s="210"/>
-      <c r="I2" s="210"/>
-      <c r="J2" s="210"/>
-      <c r="K2" s="210"/>
-      <c r="L2" s="210"/>
-      <c r="M2" s="210"/>
-      <c r="N2" s="208" t="s">
+      <c r="H2" s="223"/>
+      <c r="I2" s="223"/>
+      <c r="J2" s="223"/>
+      <c r="K2" s="223"/>
+      <c r="L2" s="223"/>
+      <c r="M2" s="223"/>
+      <c r="N2" s="225" t="s">
         <v>118</v>
       </c>
-      <c r="O2" s="208"/>
-      <c r="P2" s="208"/>
-      <c r="Q2" s="208"/>
-      <c r="R2" s="208"/>
-      <c r="S2" s="208"/>
-      <c r="T2" s="208"/>
-      <c r="U2" s="208"/>
-      <c r="V2" s="208"/>
-      <c r="W2" s="208"/>
-      <c r="X2" s="208"/>
-      <c r="Y2" s="208"/>
-      <c r="Z2" s="208"/>
-      <c r="AA2" s="208"/>
-      <c r="AB2" s="208"/>
+      <c r="O2" s="225"/>
+      <c r="P2" s="225"/>
+      <c r="Q2" s="225"/>
+      <c r="R2" s="225"/>
+      <c r="S2" s="225"/>
+      <c r="T2" s="225"/>
+      <c r="U2" s="225"/>
+      <c r="V2" s="225"/>
+      <c r="W2" s="225"/>
+      <c r="X2" s="225"/>
+      <c r="Y2" s="225"/>
+      <c r="Z2" s="225"/>
+      <c r="AA2" s="225"/>
+      <c r="AB2" s="225"/>
       <c r="AC2" s="131"/>
-      <c r="AD2" s="211" t="s">
+      <c r="AD2" s="210" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="212"/>
-      <c r="AF2" s="212"/>
-      <c r="AG2" s="212"/>
-      <c r="AH2" s="212"/>
-      <c r="AI2" s="212"/>
-      <c r="AJ2" s="212"/>
-      <c r="AK2" s="212"/>
-      <c r="AL2" s="212"/>
-      <c r="AM2" s="212"/>
-      <c r="AN2" s="212"/>
-      <c r="AO2" s="212"/>
-      <c r="AP2" s="212"/>
-      <c r="AQ2" s="212"/>
-      <c r="AR2" s="212"/>
-      <c r="AS2" s="212"/>
-      <c r="AT2" s="212"/>
-      <c r="AU2" s="212"/>
-      <c r="AV2" s="212"/>
-      <c r="AW2" s="212"/>
-      <c r="AX2" s="212"/>
-      <c r="AY2" s="212"/>
-      <c r="AZ2" s="212"/>
-      <c r="BA2" s="212"/>
-      <c r="BB2" s="212"/>
-      <c r="BC2" s="212"/>
-      <c r="BD2" s="212"/>
-      <c r="BE2" s="212"/>
-      <c r="BF2" s="212"/>
-      <c r="BG2" s="212"/>
-      <c r="BH2" s="212"/>
-      <c r="BI2" s="212"/>
-      <c r="BJ2" s="212"/>
-      <c r="BK2" s="212"/>
+      <c r="AE2" s="211"/>
+      <c r="AF2" s="211"/>
+      <c r="AG2" s="211"/>
+      <c r="AH2" s="211"/>
+      <c r="AI2" s="211"/>
+      <c r="AJ2" s="211"/>
+      <c r="AK2" s="211"/>
+      <c r="AL2" s="211"/>
+      <c r="AM2" s="211"/>
+      <c r="AN2" s="211"/>
+      <c r="AO2" s="211"/>
+      <c r="AP2" s="211"/>
+      <c r="AQ2" s="211"/>
+      <c r="AR2" s="211"/>
+      <c r="AS2" s="211"/>
+      <c r="AT2" s="211"/>
+      <c r="AU2" s="211"/>
+      <c r="AV2" s="211"/>
+      <c r="AW2" s="211"/>
+      <c r="AX2" s="211"/>
+      <c r="AY2" s="211"/>
+      <c r="AZ2" s="211"/>
+      <c r="BA2" s="211"/>
+      <c r="BB2" s="211"/>
+      <c r="BC2" s="211"/>
+      <c r="BD2" s="211"/>
+      <c r="BE2" s="211"/>
+      <c r="BF2" s="211"/>
+      <c r="BG2" s="211"/>
+      <c r="BH2" s="211"/>
+      <c r="BI2" s="211"/>
+      <c r="BJ2" s="211"/>
+      <c r="BK2" s="211"/>
       <c r="BL2" s="191"/>
       <c r="BM2" s="191"/>
       <c r="BN2" s="205"/>
@@ -2784,59 +2783,59 @@
       <c r="CD2" s="28"/>
     </row>
     <row r="3" spans="1:82" s="136" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="222" t="s">
+      <c r="A3" s="221" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="222" t="s">
+      <c r="B3" s="221" t="s">
         <v>73</v>
       </c>
       <c r="C3" s="224" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="222" t="s">
+      <c r="D3" s="221" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="222" t="s">
+      <c r="E3" s="221" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="222" t="s">
+      <c r="F3" s="221" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="210"/>
-      <c r="H3" s="210"/>
-      <c r="I3" s="210"/>
-      <c r="J3" s="210"/>
-      <c r="K3" s="210"/>
-      <c r="L3" s="210"/>
-      <c r="M3" s="210"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
+      <c r="I3" s="223"/>
+      <c r="J3" s="223"/>
+      <c r="K3" s="223"/>
+      <c r="L3" s="223"/>
+      <c r="M3" s="223"/>
       <c r="N3" s="132" t="s">
         <v>139</v>
       </c>
-      <c r="O3" s="209">
+      <c r="O3" s="226">
         <f>DATE(2017,3,11)</f>
         <v>42805</v>
       </c>
-      <c r="P3" s="208"/>
+      <c r="P3" s="225"/>
       <c r="Q3" s="132" t="s">
         <v>139</v>
       </c>
-      <c r="R3" s="209"/>
-      <c r="S3" s="208"/>
+      <c r="R3" s="226"/>
+      <c r="S3" s="225"/>
       <c r="T3" s="132" t="s">
         <v>139</v>
       </c>
-      <c r="U3" s="209"/>
-      <c r="V3" s="208"/>
+      <c r="U3" s="226"/>
+      <c r="V3" s="225"/>
       <c r="W3" s="132" t="s">
         <v>139</v>
       </c>
-      <c r="X3" s="209"/>
-      <c r="Y3" s="208"/>
+      <c r="X3" s="226"/>
+      <c r="Y3" s="225"/>
       <c r="Z3" s="132" t="s">
         <v>139</v>
       </c>
-      <c r="AA3" s="209"/>
-      <c r="AB3" s="208"/>
+      <c r="AA3" s="226"/>
+      <c r="AB3" s="225"/>
       <c r="AC3" s="122"/>
       <c r="AD3" s="14" t="s">
         <v>4</v>
@@ -3028,12 +3027,12 @@
       <c r="CD3" s="141"/>
     </row>
     <row r="4" spans="1:82" s="136" customFormat="1" ht="45.75">
-      <c r="A4" s="222"/>
-      <c r="B4" s="222"/>
+      <c r="A4" s="221"/>
+      <c r="B4" s="221"/>
       <c r="C4" s="224"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="221"/>
+      <c r="F4" s="221"/>
       <c r="G4" s="13" t="s">
         <v>121</v>
       </c>
@@ -11036,33 +11035,33 @@
       <c r="CD47"/>
     </row>
     <row r="48" spans="1:82" s="136" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="223" t="s">
+      <c r="A48" s="222" t="s">
         <v>8</v>
       </c>
-      <c r="B48" s="218" t="s">
+      <c r="B48" s="217" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="220" t="s">
+      <c r="C48" s="219" t="s">
         <v>30</v>
       </c>
-      <c r="D48" s="218" t="s">
+      <c r="D48" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="218" t="s">
+      <c r="E48" s="217" t="s">
         <v>28</v>
       </c>
-      <c r="F48" s="210" t="s">
+      <c r="F48" s="223" t="s">
         <v>29</v>
       </c>
-      <c r="G48" s="215" t="s">
+      <c r="G48" s="214" t="s">
         <v>117</v>
       </c>
-      <c r="H48" s="216"/>
-      <c r="I48" s="216"/>
-      <c r="J48" s="216"/>
-      <c r="K48" s="216"/>
-      <c r="L48" s="216"/>
-      <c r="M48" s="217"/>
+      <c r="H48" s="215"/>
+      <c r="I48" s="215"/>
+      <c r="J48" s="215"/>
+      <c r="K48" s="215"/>
+      <c r="L48" s="215"/>
+      <c r="M48" s="216"/>
       <c r="N48" s="93" t="s">
         <v>118</v>
       </c>
@@ -11236,12 +11235,12 @@
       <c r="CD48" s="141"/>
     </row>
     <row r="49" spans="1:82" s="136" customFormat="1" ht="45">
-      <c r="A49" s="223"/>
-      <c r="B49" s="219"/>
-      <c r="C49" s="221"/>
-      <c r="D49" s="219"/>
-      <c r="E49" s="219"/>
-      <c r="F49" s="210"/>
+      <c r="A49" s="222"/>
+      <c r="B49" s="218"/>
+      <c r="C49" s="220"/>
+      <c r="D49" s="218"/>
+      <c r="E49" s="218"/>
+      <c r="F49" s="223"/>
       <c r="G49" s="50" t="s">
         <v>114</v>
       </c>
@@ -18301,6 +18300,13 @@
     <sortCondition descending="1" ref="CC50:CC88"/>
   </sortState>
   <mergeCells count="23">
+    <mergeCell ref="N2:AB2"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="G2:M3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="X3:Y3"/>
     <mergeCell ref="AD2:BK2"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:Q1"/>
@@ -18317,13 +18323,6 @@
     <mergeCell ref="D48:D49"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="N2:AB2"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="G2:M3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="X3:Y3"/>
   </mergeCells>
   <conditionalFormatting sqref="CC50:CC88">
     <cfRule type="expression" dxfId="15" priority="25">
@@ -18418,264 +18417,264 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="227" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
-      <c r="G1" s="225"/>
-      <c r="H1" s="225"/>
-      <c r="I1" s="225"/>
-      <c r="J1" s="225"/>
-      <c r="K1" s="225"/>
-      <c r="L1" s="225"/>
-      <c r="M1" s="225"/>
-      <c r="N1" s="225"/>
-      <c r="O1" s="225"/>
-      <c r="P1" s="225"/>
-      <c r="Q1" s="225"/>
-      <c r="R1" s="225"/>
-      <c r="S1" s="225"/>
-      <c r="T1" s="225"/>
-      <c r="U1" s="225"/>
-      <c r="V1" s="225"/>
-      <c r="W1" s="225"/>
-      <c r="X1" s="225"/>
-      <c r="Y1" s="225"/>
-      <c r="Z1" s="225"/>
-      <c r="AA1" s="225"/>
-      <c r="AB1" s="225"/>
-      <c r="AC1" s="225"/>
-      <c r="AD1" s="225"/>
-      <c r="AE1" s="225"/>
-      <c r="AF1" s="225"/>
-      <c r="AG1" s="225"/>
-      <c r="AH1" s="225"/>
-      <c r="AI1" s="225"/>
-      <c r="AJ1" s="225"/>
-      <c r="AK1" s="225"/>
-      <c r="AL1" s="225"/>
-      <c r="AM1" s="225"/>
-      <c r="AN1" s="225"/>
-      <c r="AO1" s="225"/>
-      <c r="AP1" s="225"/>
-      <c r="AQ1" s="225"/>
-      <c r="AR1" s="225"/>
-      <c r="AS1" s="225"/>
-      <c r="AT1" s="225"/>
-      <c r="AU1" s="225"/>
-      <c r="AV1" s="225"/>
-      <c r="AW1" s="225"/>
-      <c r="AX1" s="225"/>
-      <c r="AY1" s="225"/>
-      <c r="AZ1" s="225"/>
-      <c r="BA1" s="225"/>
-      <c r="BB1" s="225"/>
-      <c r="BC1" s="225"/>
-      <c r="BD1" s="225"/>
-      <c r="BE1" s="225"/>
-      <c r="BF1" s="225"/>
-      <c r="BG1" s="225"/>
-      <c r="BH1" s="225"/>
-      <c r="BI1" s="225"/>
-      <c r="BJ1" s="225"/>
-      <c r="BK1" s="225"/>
-      <c r="BL1" s="225"/>
-      <c r="BM1" s="225"/>
-      <c r="BN1" s="225"/>
-      <c r="BO1" s="225"/>
-      <c r="BP1" s="225"/>
-      <c r="BQ1" s="225"/>
-      <c r="BR1" s="225"/>
-      <c r="BS1" s="225"/>
-      <c r="BT1" s="225"/>
-      <c r="BU1" s="225"/>
-      <c r="BV1" s="225"/>
-      <c r="BW1" s="225"/>
-      <c r="BX1" s="225"/>
-      <c r="BY1" s="225"/>
-      <c r="BZ1" s="225"/>
-      <c r="CA1" s="225"/>
-      <c r="CB1" s="225"/>
-      <c r="CC1" s="225"/>
-      <c r="CD1" s="225"/>
-      <c r="CE1" s="225"/>
-      <c r="CF1" s="225"/>
-      <c r="CG1" s="225"/>
-      <c r="CH1" s="225"/>
-      <c r="CI1" s="225"/>
-      <c r="CJ1" s="225"/>
-      <c r="CK1" s="225"/>
-      <c r="CL1" s="225"/>
-      <c r="CM1" s="225"/>
-      <c r="CN1" s="225"/>
-      <c r="CO1" s="225"/>
-      <c r="CP1" s="225"/>
-      <c r="CQ1" s="225"/>
-      <c r="CR1" s="225"/>
-      <c r="CS1" s="225"/>
-      <c r="CT1" s="225"/>
-      <c r="CU1" s="225"/>
-      <c r="CV1" s="225"/>
-      <c r="CW1" s="225"/>
-      <c r="CX1" s="225"/>
-      <c r="CY1" s="225"/>
-      <c r="CZ1" s="225"/>
-      <c r="DA1" s="225"/>
-      <c r="DB1" s="225"/>
-      <c r="DC1" s="225"/>
-      <c r="DD1" s="225"/>
-      <c r="DE1" s="225"/>
-      <c r="DF1" s="225"/>
-      <c r="DG1" s="225"/>
-      <c r="DH1" s="225"/>
-      <c r="DI1" s="225"/>
-      <c r="DJ1" s="225"/>
-      <c r="DK1" s="225"/>
-      <c r="DL1" s="225"/>
-      <c r="DM1" s="225"/>
-      <c r="DN1" s="225"/>
-      <c r="DO1" s="225"/>
-      <c r="DP1" s="225"/>
-      <c r="DQ1" s="225"/>
-      <c r="DR1" s="225"/>
-      <c r="DS1" s="225"/>
-      <c r="DT1" s="225"/>
-      <c r="DU1" s="225"/>
-      <c r="DV1" s="225"/>
-      <c r="DW1" s="225"/>
-      <c r="DX1" s="225"/>
-      <c r="DY1" s="225"/>
-      <c r="DZ1" s="225"/>
-      <c r="EA1" s="225"/>
-      <c r="EB1" s="225"/>
-      <c r="EC1" s="225"/>
-      <c r="ED1" s="225"/>
-      <c r="EE1" s="225"/>
-      <c r="EF1" s="225"/>
-      <c r="EG1" s="225"/>
-      <c r="EH1" s="225"/>
-      <c r="EI1" s="225"/>
-      <c r="EJ1" s="225"/>
-      <c r="EK1" s="225"/>
-      <c r="EL1" s="225"/>
-      <c r="EM1" s="225"/>
-      <c r="EN1" s="225"/>
-      <c r="EO1" s="225"/>
-      <c r="EP1" s="225"/>
-      <c r="EQ1" s="225"/>
-      <c r="ER1" s="225"/>
-      <c r="ES1" s="225"/>
-      <c r="ET1" s="225"/>
-      <c r="EU1" s="225"/>
-      <c r="EV1" s="225"/>
-      <c r="EW1" s="225"/>
-      <c r="EX1" s="225"/>
-      <c r="EY1" s="225"/>
-      <c r="EZ1" s="225"/>
-      <c r="FA1" s="225"/>
-      <c r="FB1" s="225"/>
-      <c r="FC1" s="225"/>
-      <c r="FD1" s="225"/>
-      <c r="FE1" s="225"/>
-      <c r="FF1" s="225"/>
-      <c r="FG1" s="225"/>
-      <c r="FH1" s="225"/>
-      <c r="FI1" s="225"/>
-      <c r="FJ1" s="225"/>
-      <c r="FK1" s="225"/>
-      <c r="FL1" s="225"/>
-      <c r="FM1" s="225"/>
-      <c r="FN1" s="225"/>
-      <c r="FO1" s="225"/>
-      <c r="FP1" s="225"/>
-      <c r="FQ1" s="225"/>
-      <c r="FR1" s="225"/>
-      <c r="FS1" s="225"/>
-      <c r="FT1" s="225"/>
-      <c r="FU1" s="225"/>
-      <c r="FV1" s="225"/>
-      <c r="FW1" s="225"/>
-      <c r="FX1" s="225"/>
-      <c r="FY1" s="225"/>
-      <c r="FZ1" s="225"/>
-      <c r="GA1" s="225"/>
-      <c r="GB1" s="225"/>
-      <c r="GC1" s="225"/>
-      <c r="GD1" s="225"/>
-      <c r="GE1" s="225"/>
-      <c r="GF1" s="225"/>
-      <c r="GG1" s="225"/>
-      <c r="GH1" s="225"/>
-      <c r="GI1" s="225"/>
-      <c r="GJ1" s="225"/>
-      <c r="GK1" s="225"/>
-      <c r="GL1" s="225"/>
-      <c r="GM1" s="225"/>
-      <c r="GN1" s="225"/>
-      <c r="GO1" s="225"/>
-      <c r="GP1" s="225"/>
-      <c r="GQ1" s="225"/>
-      <c r="GR1" s="225"/>
-      <c r="GS1" s="225"/>
-      <c r="GT1" s="225"/>
-      <c r="GU1" s="225"/>
-      <c r="GV1" s="225"/>
-      <c r="GW1" s="225"/>
-      <c r="GX1" s="225"/>
-      <c r="GY1" s="225"/>
-      <c r="GZ1" s="225"/>
-      <c r="HA1" s="225"/>
-      <c r="HB1" s="225"/>
-      <c r="HC1" s="225"/>
-      <c r="HD1" s="225"/>
-      <c r="HE1" s="225"/>
-      <c r="HF1" s="225"/>
-      <c r="HG1" s="225"/>
-      <c r="HH1" s="225"/>
-      <c r="HI1" s="225"/>
-      <c r="HJ1" s="225"/>
-      <c r="HK1" s="225"/>
-      <c r="HL1" s="225"/>
-      <c r="HM1" s="225"/>
-      <c r="HN1" s="225"/>
-      <c r="HO1" s="225"/>
-      <c r="HP1" s="225"/>
-      <c r="HQ1" s="225"/>
-      <c r="HR1" s="225"/>
-      <c r="HS1" s="225"/>
-      <c r="HT1" s="225"/>
-      <c r="HU1" s="225"/>
-      <c r="HV1" s="225"/>
-      <c r="HW1" s="225"/>
-      <c r="HX1" s="225"/>
-      <c r="HY1" s="225"/>
-      <c r="HZ1" s="225"/>
-      <c r="IA1" s="225"/>
-      <c r="IB1" s="225"/>
-      <c r="IC1" s="225"/>
-      <c r="ID1" s="225"/>
-      <c r="IE1" s="225"/>
-      <c r="IF1" s="225"/>
-      <c r="IG1" s="225"/>
-      <c r="IH1" s="225"/>
-      <c r="II1" s="225"/>
-      <c r="IJ1" s="225"/>
-      <c r="IK1" s="225"/>
-      <c r="IL1" s="225"/>
-      <c r="IM1" s="225"/>
-      <c r="IN1" s="225"/>
-      <c r="IO1" s="225"/>
-      <c r="IP1" s="225"/>
-      <c r="IQ1" s="225"/>
-      <c r="IR1" s="225"/>
-      <c r="IS1" s="225"/>
-      <c r="IT1" s="225"/>
-      <c r="IU1" s="225"/>
-      <c r="IV1" s="225"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+      <c r="H1" s="227"/>
+      <c r="I1" s="227"/>
+      <c r="J1" s="227"/>
+      <c r="K1" s="227"/>
+      <c r="L1" s="227"/>
+      <c r="M1" s="227"/>
+      <c r="N1" s="227"/>
+      <c r="O1" s="227"/>
+      <c r="P1" s="227"/>
+      <c r="Q1" s="227"/>
+      <c r="R1" s="227"/>
+      <c r="S1" s="227"/>
+      <c r="T1" s="227"/>
+      <c r="U1" s="227"/>
+      <c r="V1" s="227"/>
+      <c r="W1" s="227"/>
+      <c r="X1" s="227"/>
+      <c r="Y1" s="227"/>
+      <c r="Z1" s="227"/>
+      <c r="AA1" s="227"/>
+      <c r="AB1" s="227"/>
+      <c r="AC1" s="227"/>
+      <c r="AD1" s="227"/>
+      <c r="AE1" s="227"/>
+      <c r="AF1" s="227"/>
+      <c r="AG1" s="227"/>
+      <c r="AH1" s="227"/>
+      <c r="AI1" s="227"/>
+      <c r="AJ1" s="227"/>
+      <c r="AK1" s="227"/>
+      <c r="AL1" s="227"/>
+      <c r="AM1" s="227"/>
+      <c r="AN1" s="227"/>
+      <c r="AO1" s="227"/>
+      <c r="AP1" s="227"/>
+      <c r="AQ1" s="227"/>
+      <c r="AR1" s="227"/>
+      <c r="AS1" s="227"/>
+      <c r="AT1" s="227"/>
+      <c r="AU1" s="227"/>
+      <c r="AV1" s="227"/>
+      <c r="AW1" s="227"/>
+      <c r="AX1" s="227"/>
+      <c r="AY1" s="227"/>
+      <c r="AZ1" s="227"/>
+      <c r="BA1" s="227"/>
+      <c r="BB1" s="227"/>
+      <c r="BC1" s="227"/>
+      <c r="BD1" s="227"/>
+      <c r="BE1" s="227"/>
+      <c r="BF1" s="227"/>
+      <c r="BG1" s="227"/>
+      <c r="BH1" s="227"/>
+      <c r="BI1" s="227"/>
+      <c r="BJ1" s="227"/>
+      <c r="BK1" s="227"/>
+      <c r="BL1" s="227"/>
+      <c r="BM1" s="227"/>
+      <c r="BN1" s="227"/>
+      <c r="BO1" s="227"/>
+      <c r="BP1" s="227"/>
+      <c r="BQ1" s="227"/>
+      <c r="BR1" s="227"/>
+      <c r="BS1" s="227"/>
+      <c r="BT1" s="227"/>
+      <c r="BU1" s="227"/>
+      <c r="BV1" s="227"/>
+      <c r="BW1" s="227"/>
+      <c r="BX1" s="227"/>
+      <c r="BY1" s="227"/>
+      <c r="BZ1" s="227"/>
+      <c r="CA1" s="227"/>
+      <c r="CB1" s="227"/>
+      <c r="CC1" s="227"/>
+      <c r="CD1" s="227"/>
+      <c r="CE1" s="227"/>
+      <c r="CF1" s="227"/>
+      <c r="CG1" s="227"/>
+      <c r="CH1" s="227"/>
+      <c r="CI1" s="227"/>
+      <c r="CJ1" s="227"/>
+      <c r="CK1" s="227"/>
+      <c r="CL1" s="227"/>
+      <c r="CM1" s="227"/>
+      <c r="CN1" s="227"/>
+      <c r="CO1" s="227"/>
+      <c r="CP1" s="227"/>
+      <c r="CQ1" s="227"/>
+      <c r="CR1" s="227"/>
+      <c r="CS1" s="227"/>
+      <c r="CT1" s="227"/>
+      <c r="CU1" s="227"/>
+      <c r="CV1" s="227"/>
+      <c r="CW1" s="227"/>
+      <c r="CX1" s="227"/>
+      <c r="CY1" s="227"/>
+      <c r="CZ1" s="227"/>
+      <c r="DA1" s="227"/>
+      <c r="DB1" s="227"/>
+      <c r="DC1" s="227"/>
+      <c r="DD1" s="227"/>
+      <c r="DE1" s="227"/>
+      <c r="DF1" s="227"/>
+      <c r="DG1" s="227"/>
+      <c r="DH1" s="227"/>
+      <c r="DI1" s="227"/>
+      <c r="DJ1" s="227"/>
+      <c r="DK1" s="227"/>
+      <c r="DL1" s="227"/>
+      <c r="DM1" s="227"/>
+      <c r="DN1" s="227"/>
+      <c r="DO1" s="227"/>
+      <c r="DP1" s="227"/>
+      <c r="DQ1" s="227"/>
+      <c r="DR1" s="227"/>
+      <c r="DS1" s="227"/>
+      <c r="DT1" s="227"/>
+      <c r="DU1" s="227"/>
+      <c r="DV1" s="227"/>
+      <c r="DW1" s="227"/>
+      <c r="DX1" s="227"/>
+      <c r="DY1" s="227"/>
+      <c r="DZ1" s="227"/>
+      <c r="EA1" s="227"/>
+      <c r="EB1" s="227"/>
+      <c r="EC1" s="227"/>
+      <c r="ED1" s="227"/>
+      <c r="EE1" s="227"/>
+      <c r="EF1" s="227"/>
+      <c r="EG1" s="227"/>
+      <c r="EH1" s="227"/>
+      <c r="EI1" s="227"/>
+      <c r="EJ1" s="227"/>
+      <c r="EK1" s="227"/>
+      <c r="EL1" s="227"/>
+      <c r="EM1" s="227"/>
+      <c r="EN1" s="227"/>
+      <c r="EO1" s="227"/>
+      <c r="EP1" s="227"/>
+      <c r="EQ1" s="227"/>
+      <c r="ER1" s="227"/>
+      <c r="ES1" s="227"/>
+      <c r="ET1" s="227"/>
+      <c r="EU1" s="227"/>
+      <c r="EV1" s="227"/>
+      <c r="EW1" s="227"/>
+      <c r="EX1" s="227"/>
+      <c r="EY1" s="227"/>
+      <c r="EZ1" s="227"/>
+      <c r="FA1" s="227"/>
+      <c r="FB1" s="227"/>
+      <c r="FC1" s="227"/>
+      <c r="FD1" s="227"/>
+      <c r="FE1" s="227"/>
+      <c r="FF1" s="227"/>
+      <c r="FG1" s="227"/>
+      <c r="FH1" s="227"/>
+      <c r="FI1" s="227"/>
+      <c r="FJ1" s="227"/>
+      <c r="FK1" s="227"/>
+      <c r="FL1" s="227"/>
+      <c r="FM1" s="227"/>
+      <c r="FN1" s="227"/>
+      <c r="FO1" s="227"/>
+      <c r="FP1" s="227"/>
+      <c r="FQ1" s="227"/>
+      <c r="FR1" s="227"/>
+      <c r="FS1" s="227"/>
+      <c r="FT1" s="227"/>
+      <c r="FU1" s="227"/>
+      <c r="FV1" s="227"/>
+      <c r="FW1" s="227"/>
+      <c r="FX1" s="227"/>
+      <c r="FY1" s="227"/>
+      <c r="FZ1" s="227"/>
+      <c r="GA1" s="227"/>
+      <c r="GB1" s="227"/>
+      <c r="GC1" s="227"/>
+      <c r="GD1" s="227"/>
+      <c r="GE1" s="227"/>
+      <c r="GF1" s="227"/>
+      <c r="GG1" s="227"/>
+      <c r="GH1" s="227"/>
+      <c r="GI1" s="227"/>
+      <c r="GJ1" s="227"/>
+      <c r="GK1" s="227"/>
+      <c r="GL1" s="227"/>
+      <c r="GM1" s="227"/>
+      <c r="GN1" s="227"/>
+      <c r="GO1" s="227"/>
+      <c r="GP1" s="227"/>
+      <c r="GQ1" s="227"/>
+      <c r="GR1" s="227"/>
+      <c r="GS1" s="227"/>
+      <c r="GT1" s="227"/>
+      <c r="GU1" s="227"/>
+      <c r="GV1" s="227"/>
+      <c r="GW1" s="227"/>
+      <c r="GX1" s="227"/>
+      <c r="GY1" s="227"/>
+      <c r="GZ1" s="227"/>
+      <c r="HA1" s="227"/>
+      <c r="HB1" s="227"/>
+      <c r="HC1" s="227"/>
+      <c r="HD1" s="227"/>
+      <c r="HE1" s="227"/>
+      <c r="HF1" s="227"/>
+      <c r="HG1" s="227"/>
+      <c r="HH1" s="227"/>
+      <c r="HI1" s="227"/>
+      <c r="HJ1" s="227"/>
+      <c r="HK1" s="227"/>
+      <c r="HL1" s="227"/>
+      <c r="HM1" s="227"/>
+      <c r="HN1" s="227"/>
+      <c r="HO1" s="227"/>
+      <c r="HP1" s="227"/>
+      <c r="HQ1" s="227"/>
+      <c r="HR1" s="227"/>
+      <c r="HS1" s="227"/>
+      <c r="HT1" s="227"/>
+      <c r="HU1" s="227"/>
+      <c r="HV1" s="227"/>
+      <c r="HW1" s="227"/>
+      <c r="HX1" s="227"/>
+      <c r="HY1" s="227"/>
+      <c r="HZ1" s="227"/>
+      <c r="IA1" s="227"/>
+      <c r="IB1" s="227"/>
+      <c r="IC1" s="227"/>
+      <c r="ID1" s="227"/>
+      <c r="IE1" s="227"/>
+      <c r="IF1" s="227"/>
+      <c r="IG1" s="227"/>
+      <c r="IH1" s="227"/>
+      <c r="II1" s="227"/>
+      <c r="IJ1" s="227"/>
+      <c r="IK1" s="227"/>
+      <c r="IL1" s="227"/>
+      <c r="IM1" s="227"/>
+      <c r="IN1" s="227"/>
+      <c r="IO1" s="227"/>
+      <c r="IP1" s="227"/>
+      <c r="IQ1" s="227"/>
+      <c r="IR1" s="227"/>
+      <c r="IS1" s="227"/>
+      <c r="IT1" s="227"/>
+      <c r="IU1" s="227"/>
+      <c r="IV1" s="227"/>
     </row>
     <row r="2" spans="1:256" s="29" customFormat="1">
       <c r="A2" s="14" t="s">
@@ -45584,358 +45583,358 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="227" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
-      <c r="G1" s="225"/>
-      <c r="H1" s="225"/>
-      <c r="I1" s="225"/>
-      <c r="J1" s="225"/>
-      <c r="K1" s="225"/>
-      <c r="L1" s="225"/>
-      <c r="M1" s="225"/>
-      <c r="N1" s="225"/>
-      <c r="O1" s="225"/>
-      <c r="P1" s="225"/>
-      <c r="Q1" s="225"/>
-      <c r="R1" s="225"/>
-      <c r="S1" s="225"/>
-      <c r="T1" s="225"/>
-      <c r="U1" s="225"/>
-      <c r="V1" s="225"/>
-      <c r="W1" s="225"/>
-      <c r="X1" s="225"/>
-      <c r="Y1" s="225"/>
-      <c r="Z1" s="225"/>
-      <c r="AA1" s="225"/>
-      <c r="AB1" s="225"/>
-      <c r="AC1" s="225"/>
-      <c r="AD1" s="225"/>
-      <c r="AE1" s="225"/>
-      <c r="AF1" s="225"/>
-      <c r="AG1" s="225"/>
-      <c r="AH1" s="225"/>
-      <c r="AI1" s="225"/>
-      <c r="AJ1" s="225"/>
-      <c r="AK1" s="225"/>
-      <c r="AL1" s="225"/>
-      <c r="AM1" s="225"/>
-      <c r="AN1" s="225"/>
-      <c r="AO1" s="225"/>
-      <c r="AP1" s="225"/>
-      <c r="AQ1" s="225"/>
-      <c r="AR1" s="225"/>
-      <c r="AS1" s="225"/>
-      <c r="AT1" s="225"/>
-      <c r="AU1" s="225"/>
-      <c r="AV1" s="225"/>
-      <c r="AW1" s="225"/>
-      <c r="AX1" s="225"/>
-      <c r="AY1" s="225"/>
-      <c r="AZ1" s="225"/>
-      <c r="BA1" s="225"/>
-      <c r="BB1" s="225"/>
-      <c r="BC1" s="225"/>
-      <c r="BD1" s="225"/>
-      <c r="BE1" s="225"/>
-      <c r="BF1" s="225"/>
-      <c r="BG1" s="225"/>
-      <c r="BH1" s="225"/>
-      <c r="BI1" s="225"/>
-      <c r="BJ1" s="225"/>
-      <c r="BK1" s="225"/>
-      <c r="BL1" s="225"/>
-      <c r="BM1" s="225"/>
-      <c r="BN1" s="225"/>
-      <c r="BO1" s="225"/>
-      <c r="BP1" s="225"/>
-      <c r="BQ1" s="225"/>
-      <c r="BR1" s="225"/>
-      <c r="BS1" s="225"/>
-      <c r="BT1" s="225"/>
-      <c r="BU1" s="225"/>
-      <c r="BV1" s="225"/>
-      <c r="BW1" s="225"/>
-      <c r="BX1" s="225"/>
-      <c r="BY1" s="225"/>
-      <c r="BZ1" s="225"/>
-      <c r="CA1" s="225"/>
-      <c r="CB1" s="225"/>
-      <c r="CC1" s="225"/>
-      <c r="CD1" s="225"/>
-      <c r="CE1" s="225"/>
-      <c r="CF1" s="225"/>
-      <c r="CG1" s="225"/>
-      <c r="CH1" s="225"/>
-      <c r="CI1" s="225"/>
-      <c r="CJ1" s="225"/>
-      <c r="CK1" s="225"/>
-      <c r="CL1" s="225"/>
-      <c r="CM1" s="225"/>
-      <c r="CN1" s="225"/>
-      <c r="CO1" s="225"/>
-      <c r="CP1" s="225"/>
-      <c r="CQ1" s="225"/>
-      <c r="CR1" s="225"/>
-      <c r="CS1" s="225"/>
-      <c r="CT1" s="225"/>
-      <c r="CU1" s="225"/>
-      <c r="CV1" s="225"/>
-      <c r="CW1" s="225"/>
-      <c r="CX1" s="225"/>
-      <c r="CY1" s="225"/>
-      <c r="CZ1" s="225"/>
-      <c r="DA1" s="225"/>
-      <c r="DB1" s="225"/>
-      <c r="DC1" s="225"/>
-      <c r="DD1" s="225"/>
-      <c r="DE1" s="225"/>
-      <c r="DF1" s="225"/>
-      <c r="DG1" s="225"/>
-      <c r="DH1" s="225"/>
-      <c r="DI1" s="225"/>
-      <c r="DJ1" s="225"/>
-      <c r="DK1" s="225"/>
-      <c r="DL1" s="225"/>
-      <c r="DM1" s="225"/>
-      <c r="DN1" s="225"/>
-      <c r="DO1" s="225"/>
-      <c r="DP1" s="225"/>
-      <c r="DQ1" s="225"/>
-      <c r="DR1" s="225"/>
-      <c r="DS1" s="225"/>
-      <c r="DT1" s="225"/>
-      <c r="DU1" s="225"/>
-      <c r="DV1" s="225"/>
-      <c r="DW1" s="225"/>
-      <c r="DX1" s="225"/>
-      <c r="DY1" s="225"/>
-      <c r="DZ1" s="225"/>
-      <c r="EA1" s="225"/>
-      <c r="EB1" s="225"/>
-      <c r="EC1" s="225"/>
-      <c r="ED1" s="225"/>
-      <c r="EE1" s="225"/>
-      <c r="EF1" s="225"/>
-      <c r="EG1" s="225"/>
-      <c r="EH1" s="225"/>
-      <c r="EI1" s="225"/>
-      <c r="EJ1" s="225"/>
-      <c r="EK1" s="225"/>
-      <c r="EL1" s="225"/>
-      <c r="EM1" s="225"/>
-      <c r="EN1" s="225"/>
-      <c r="EO1" s="225"/>
-      <c r="EP1" s="225"/>
-      <c r="EQ1" s="225"/>
-      <c r="ER1" s="225"/>
-      <c r="ES1" s="225"/>
-      <c r="ET1" s="225"/>
-      <c r="EU1" s="225"/>
-      <c r="EV1" s="225"/>
-      <c r="EW1" s="225"/>
-      <c r="EX1" s="225"/>
-      <c r="EY1" s="225"/>
-      <c r="EZ1" s="225"/>
-      <c r="FA1" s="225"/>
-      <c r="FB1" s="225"/>
-      <c r="FC1" s="225"/>
-      <c r="FD1" s="225"/>
-      <c r="FE1" s="225"/>
-      <c r="FF1" s="225"/>
-      <c r="FG1" s="225"/>
-      <c r="FH1" s="225"/>
-      <c r="FI1" s="225"/>
-      <c r="FJ1" s="225"/>
-      <c r="FK1" s="225"/>
-      <c r="FL1" s="225"/>
-      <c r="FM1" s="225"/>
-      <c r="FN1" s="225"/>
-      <c r="FO1" s="225"/>
-      <c r="FP1" s="225"/>
-      <c r="FQ1" s="225"/>
-      <c r="FR1" s="225"/>
-      <c r="FS1" s="225"/>
-      <c r="FT1" s="225"/>
-      <c r="FU1" s="225"/>
-      <c r="FV1" s="225"/>
-      <c r="FW1" s="225"/>
-      <c r="FX1" s="225"/>
-      <c r="FY1" s="225"/>
-      <c r="FZ1" s="225"/>
-      <c r="GA1" s="225"/>
-      <c r="GB1" s="225"/>
-      <c r="GC1" s="225"/>
-      <c r="GD1" s="225"/>
-      <c r="GE1" s="225"/>
-      <c r="GF1" s="225"/>
-      <c r="GG1" s="225"/>
-      <c r="GH1" s="225"/>
-      <c r="GI1" s="225"/>
-      <c r="GJ1" s="225"/>
-      <c r="GK1" s="225"/>
-      <c r="GL1" s="225"/>
-      <c r="GM1" s="225"/>
-      <c r="GN1" s="225"/>
-      <c r="GO1" s="225"/>
-      <c r="GP1" s="225"/>
-      <c r="GQ1" s="225"/>
-      <c r="GR1" s="225"/>
-      <c r="GS1" s="225"/>
-      <c r="GT1" s="225"/>
-      <c r="GU1" s="225"/>
-      <c r="GV1" s="225"/>
-      <c r="GW1" s="225"/>
-      <c r="GX1" s="225"/>
-      <c r="GY1" s="225"/>
-      <c r="GZ1" s="225"/>
-      <c r="HA1" s="225"/>
-      <c r="HB1" s="225"/>
-      <c r="HC1" s="225"/>
-      <c r="HD1" s="225"/>
-      <c r="HE1" s="225"/>
-      <c r="HF1" s="225"/>
-      <c r="HG1" s="225"/>
-      <c r="HH1" s="225"/>
-      <c r="HI1" s="225"/>
-      <c r="HJ1" s="225"/>
-      <c r="HK1" s="225"/>
-      <c r="HL1" s="225"/>
-      <c r="HM1" s="225"/>
-      <c r="HN1" s="225"/>
-      <c r="HO1" s="225"/>
-      <c r="HP1" s="225"/>
-      <c r="HQ1" s="225"/>
-      <c r="HR1" s="225"/>
-      <c r="HS1" s="225"/>
-      <c r="HT1" s="225"/>
-      <c r="HU1" s="225"/>
-      <c r="HV1" s="225"/>
-      <c r="HW1" s="225"/>
-      <c r="HX1" s="225"/>
-      <c r="HY1" s="225"/>
-      <c r="HZ1" s="225"/>
-      <c r="IA1" s="225"/>
-      <c r="IB1" s="225"/>
-      <c r="IC1" s="225"/>
-      <c r="ID1" s="225"/>
-      <c r="IE1" s="225"/>
-      <c r="IF1" s="225"/>
-      <c r="IG1" s="225"/>
-      <c r="IH1" s="225"/>
-      <c r="II1" s="225"/>
-      <c r="IJ1" s="225"/>
-      <c r="IK1" s="225"/>
-      <c r="IL1" s="225"/>
-      <c r="IM1" s="225"/>
-      <c r="IN1" s="225"/>
-      <c r="IO1" s="225"/>
-      <c r="IP1" s="225"/>
-      <c r="IQ1" s="225"/>
-      <c r="IR1" s="225"/>
-      <c r="IS1" s="225"/>
-      <c r="IT1" s="225"/>
-      <c r="IU1" s="225"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+      <c r="H1" s="227"/>
+      <c r="I1" s="227"/>
+      <c r="J1" s="227"/>
+      <c r="K1" s="227"/>
+      <c r="L1" s="227"/>
+      <c r="M1" s="227"/>
+      <c r="N1" s="227"/>
+      <c r="O1" s="227"/>
+      <c r="P1" s="227"/>
+      <c r="Q1" s="227"/>
+      <c r="R1" s="227"/>
+      <c r="S1" s="227"/>
+      <c r="T1" s="227"/>
+      <c r="U1" s="227"/>
+      <c r="V1" s="227"/>
+      <c r="W1" s="227"/>
+      <c r="X1" s="227"/>
+      <c r="Y1" s="227"/>
+      <c r="Z1" s="227"/>
+      <c r="AA1" s="227"/>
+      <c r="AB1" s="227"/>
+      <c r="AC1" s="227"/>
+      <c r="AD1" s="227"/>
+      <c r="AE1" s="227"/>
+      <c r="AF1" s="227"/>
+      <c r="AG1" s="227"/>
+      <c r="AH1" s="227"/>
+      <c r="AI1" s="227"/>
+      <c r="AJ1" s="227"/>
+      <c r="AK1" s="227"/>
+      <c r="AL1" s="227"/>
+      <c r="AM1" s="227"/>
+      <c r="AN1" s="227"/>
+      <c r="AO1" s="227"/>
+      <c r="AP1" s="227"/>
+      <c r="AQ1" s="227"/>
+      <c r="AR1" s="227"/>
+      <c r="AS1" s="227"/>
+      <c r="AT1" s="227"/>
+      <c r="AU1" s="227"/>
+      <c r="AV1" s="227"/>
+      <c r="AW1" s="227"/>
+      <c r="AX1" s="227"/>
+      <c r="AY1" s="227"/>
+      <c r="AZ1" s="227"/>
+      <c r="BA1" s="227"/>
+      <c r="BB1" s="227"/>
+      <c r="BC1" s="227"/>
+      <c r="BD1" s="227"/>
+      <c r="BE1" s="227"/>
+      <c r="BF1" s="227"/>
+      <c r="BG1" s="227"/>
+      <c r="BH1" s="227"/>
+      <c r="BI1" s="227"/>
+      <c r="BJ1" s="227"/>
+      <c r="BK1" s="227"/>
+      <c r="BL1" s="227"/>
+      <c r="BM1" s="227"/>
+      <c r="BN1" s="227"/>
+      <c r="BO1" s="227"/>
+      <c r="BP1" s="227"/>
+      <c r="BQ1" s="227"/>
+      <c r="BR1" s="227"/>
+      <c r="BS1" s="227"/>
+      <c r="BT1" s="227"/>
+      <c r="BU1" s="227"/>
+      <c r="BV1" s="227"/>
+      <c r="BW1" s="227"/>
+      <c r="BX1" s="227"/>
+      <c r="BY1" s="227"/>
+      <c r="BZ1" s="227"/>
+      <c r="CA1" s="227"/>
+      <c r="CB1" s="227"/>
+      <c r="CC1" s="227"/>
+      <c r="CD1" s="227"/>
+      <c r="CE1" s="227"/>
+      <c r="CF1" s="227"/>
+      <c r="CG1" s="227"/>
+      <c r="CH1" s="227"/>
+      <c r="CI1" s="227"/>
+      <c r="CJ1" s="227"/>
+      <c r="CK1" s="227"/>
+      <c r="CL1" s="227"/>
+      <c r="CM1" s="227"/>
+      <c r="CN1" s="227"/>
+      <c r="CO1" s="227"/>
+      <c r="CP1" s="227"/>
+      <c r="CQ1" s="227"/>
+      <c r="CR1" s="227"/>
+      <c r="CS1" s="227"/>
+      <c r="CT1" s="227"/>
+      <c r="CU1" s="227"/>
+      <c r="CV1" s="227"/>
+      <c r="CW1" s="227"/>
+      <c r="CX1" s="227"/>
+      <c r="CY1" s="227"/>
+      <c r="CZ1" s="227"/>
+      <c r="DA1" s="227"/>
+      <c r="DB1" s="227"/>
+      <c r="DC1" s="227"/>
+      <c r="DD1" s="227"/>
+      <c r="DE1" s="227"/>
+      <c r="DF1" s="227"/>
+      <c r="DG1" s="227"/>
+      <c r="DH1" s="227"/>
+      <c r="DI1" s="227"/>
+      <c r="DJ1" s="227"/>
+      <c r="DK1" s="227"/>
+      <c r="DL1" s="227"/>
+      <c r="DM1" s="227"/>
+      <c r="DN1" s="227"/>
+      <c r="DO1" s="227"/>
+      <c r="DP1" s="227"/>
+      <c r="DQ1" s="227"/>
+      <c r="DR1" s="227"/>
+      <c r="DS1" s="227"/>
+      <c r="DT1" s="227"/>
+      <c r="DU1" s="227"/>
+      <c r="DV1" s="227"/>
+      <c r="DW1" s="227"/>
+      <c r="DX1" s="227"/>
+      <c r="DY1" s="227"/>
+      <c r="DZ1" s="227"/>
+      <c r="EA1" s="227"/>
+      <c r="EB1" s="227"/>
+      <c r="EC1" s="227"/>
+      <c r="ED1" s="227"/>
+      <c r="EE1" s="227"/>
+      <c r="EF1" s="227"/>
+      <c r="EG1" s="227"/>
+      <c r="EH1" s="227"/>
+      <c r="EI1" s="227"/>
+      <c r="EJ1" s="227"/>
+      <c r="EK1" s="227"/>
+      <c r="EL1" s="227"/>
+      <c r="EM1" s="227"/>
+      <c r="EN1" s="227"/>
+      <c r="EO1" s="227"/>
+      <c r="EP1" s="227"/>
+      <c r="EQ1" s="227"/>
+      <c r="ER1" s="227"/>
+      <c r="ES1" s="227"/>
+      <c r="ET1" s="227"/>
+      <c r="EU1" s="227"/>
+      <c r="EV1" s="227"/>
+      <c r="EW1" s="227"/>
+      <c r="EX1" s="227"/>
+      <c r="EY1" s="227"/>
+      <c r="EZ1" s="227"/>
+      <c r="FA1" s="227"/>
+      <c r="FB1" s="227"/>
+      <c r="FC1" s="227"/>
+      <c r="FD1" s="227"/>
+      <c r="FE1" s="227"/>
+      <c r="FF1" s="227"/>
+      <c r="FG1" s="227"/>
+      <c r="FH1" s="227"/>
+      <c r="FI1" s="227"/>
+      <c r="FJ1" s="227"/>
+      <c r="FK1" s="227"/>
+      <c r="FL1" s="227"/>
+      <c r="FM1" s="227"/>
+      <c r="FN1" s="227"/>
+      <c r="FO1" s="227"/>
+      <c r="FP1" s="227"/>
+      <c r="FQ1" s="227"/>
+      <c r="FR1" s="227"/>
+      <c r="FS1" s="227"/>
+      <c r="FT1" s="227"/>
+      <c r="FU1" s="227"/>
+      <c r="FV1" s="227"/>
+      <c r="FW1" s="227"/>
+      <c r="FX1" s="227"/>
+      <c r="FY1" s="227"/>
+      <c r="FZ1" s="227"/>
+      <c r="GA1" s="227"/>
+      <c r="GB1" s="227"/>
+      <c r="GC1" s="227"/>
+      <c r="GD1" s="227"/>
+      <c r="GE1" s="227"/>
+      <c r="GF1" s="227"/>
+      <c r="GG1" s="227"/>
+      <c r="GH1" s="227"/>
+      <c r="GI1" s="227"/>
+      <c r="GJ1" s="227"/>
+      <c r="GK1" s="227"/>
+      <c r="GL1" s="227"/>
+      <c r="GM1" s="227"/>
+      <c r="GN1" s="227"/>
+      <c r="GO1" s="227"/>
+      <c r="GP1" s="227"/>
+      <c r="GQ1" s="227"/>
+      <c r="GR1" s="227"/>
+      <c r="GS1" s="227"/>
+      <c r="GT1" s="227"/>
+      <c r="GU1" s="227"/>
+      <c r="GV1" s="227"/>
+      <c r="GW1" s="227"/>
+      <c r="GX1" s="227"/>
+      <c r="GY1" s="227"/>
+      <c r="GZ1" s="227"/>
+      <c r="HA1" s="227"/>
+      <c r="HB1" s="227"/>
+      <c r="HC1" s="227"/>
+      <c r="HD1" s="227"/>
+      <c r="HE1" s="227"/>
+      <c r="HF1" s="227"/>
+      <c r="HG1" s="227"/>
+      <c r="HH1" s="227"/>
+      <c r="HI1" s="227"/>
+      <c r="HJ1" s="227"/>
+      <c r="HK1" s="227"/>
+      <c r="HL1" s="227"/>
+      <c r="HM1" s="227"/>
+      <c r="HN1" s="227"/>
+      <c r="HO1" s="227"/>
+      <c r="HP1" s="227"/>
+      <c r="HQ1" s="227"/>
+      <c r="HR1" s="227"/>
+      <c r="HS1" s="227"/>
+      <c r="HT1" s="227"/>
+      <c r="HU1" s="227"/>
+      <c r="HV1" s="227"/>
+      <c r="HW1" s="227"/>
+      <c r="HX1" s="227"/>
+      <c r="HY1" s="227"/>
+      <c r="HZ1" s="227"/>
+      <c r="IA1" s="227"/>
+      <c r="IB1" s="227"/>
+      <c r="IC1" s="227"/>
+      <c r="ID1" s="227"/>
+      <c r="IE1" s="227"/>
+      <c r="IF1" s="227"/>
+      <c r="IG1" s="227"/>
+      <c r="IH1" s="227"/>
+      <c r="II1" s="227"/>
+      <c r="IJ1" s="227"/>
+      <c r="IK1" s="227"/>
+      <c r="IL1" s="227"/>
+      <c r="IM1" s="227"/>
+      <c r="IN1" s="227"/>
+      <c r="IO1" s="227"/>
+      <c r="IP1" s="227"/>
+      <c r="IQ1" s="227"/>
+      <c r="IR1" s="227"/>
+      <c r="IS1" s="227"/>
+      <c r="IT1" s="227"/>
+      <c r="IU1" s="227"/>
     </row>
     <row r="2" spans="1:255" ht="15.75" thickBot="1">
-      <c r="A2" s="228" t="str">
+      <c r="A2" s="230" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
     </row>
     <row r="3" spans="1:255" ht="15" customHeight="1">
-      <c r="A3" s="229" t="str">
+      <c r="A3" s="231" t="str">
         <f>'Сводная таблица'!A3:A4</f>
         <v>№ п/п</v>
       </c>
-      <c r="B3" s="231" t="str">
+      <c r="B3" s="233" t="str">
         <f>'Сводная таблица'!B3:B4</f>
         <v>группа</v>
       </c>
-      <c r="C3" s="233" t="str">
+      <c r="C3" s="235" t="str">
         <f>'Сводная таблица'!C3:C4</f>
         <v>подргуппа</v>
       </c>
-      <c r="D3" s="235" t="str">
+      <c r="D3" s="237" t="str">
         <f>'Сводная таблица'!D3:D4</f>
         <v>Фамилия</v>
       </c>
-      <c r="E3" s="237" t="str">
+      <c r="E3" s="239" t="str">
         <f>'Сводная таблица'!E3:E4</f>
         <v>Имя</v>
       </c>
-      <c r="F3" s="226" t="str">
+      <c r="F3" s="228" t="str">
         <f>'Сводная таблица'!F3:F4</f>
         <v>Отчество</v>
       </c>
-      <c r="G3" s="229" t="s">
+      <c r="G3" s="231" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="235" t="s">
+      <c r="H3" s="237" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="242" t="s">
+      <c r="I3" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="242" t="s">
+      <c r="J3" s="244" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="239" t="s">
+      <c r="K3" s="241" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="244" t="s">
+      <c r="L3" s="246" t="s">
         <v>140</v>
       </c>
-      <c r="M3" s="208" t="s">
+      <c r="M3" s="225" t="s">
         <v>163</v>
       </c>
-      <c r="N3" s="208"/>
-      <c r="O3" s="208"/>
-      <c r="P3" s="208"/>
-      <c r="Q3" s="208"/>
-      <c r="R3" s="208"/>
-      <c r="S3" s="208"/>
-      <c r="T3" s="208"/>
-      <c r="U3" s="208"/>
-      <c r="V3" s="208"/>
-      <c r="W3" s="208"/>
-      <c r="X3" s="208"/>
-      <c r="Y3" s="208"/>
-      <c r="Z3" s="208"/>
-      <c r="AA3" s="208"/>
-      <c r="AB3" s="208"/>
-      <c r="AC3" s="208"/>
-      <c r="AD3" s="208"/>
-      <c r="AE3" s="208"/>
+      <c r="N3" s="225"/>
+      <c r="O3" s="225"/>
+      <c r="P3" s="225"/>
+      <c r="Q3" s="225"/>
+      <c r="R3" s="225"/>
+      <c r="S3" s="225"/>
+      <c r="T3" s="225"/>
+      <c r="U3" s="225"/>
+      <c r="V3" s="225"/>
+      <c r="W3" s="225"/>
+      <c r="X3" s="225"/>
+      <c r="Y3" s="225"/>
+      <c r="Z3" s="225"/>
+      <c r="AA3" s="225"/>
+      <c r="AB3" s="225"/>
+      <c r="AC3" s="225"/>
+      <c r="AD3" s="225"/>
+      <c r="AE3" s="225"/>
     </row>
     <row r="4" spans="1:255" ht="15.75" thickBot="1">
-      <c r="A4" s="230"/>
-      <c r="B4" s="232"/>
-      <c r="C4" s="234"/>
-      <c r="D4" s="236"/>
-      <c r="E4" s="238"/>
-      <c r="F4" s="227"/>
-      <c r="G4" s="241"/>
-      <c r="H4" s="218"/>
-      <c r="I4" s="243"/>
-      <c r="J4" s="243"/>
-      <c r="K4" s="240"/>
-      <c r="L4" s="245"/>
+      <c r="A4" s="232"/>
+      <c r="B4" s="234"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="238"/>
+      <c r="E4" s="240"/>
+      <c r="F4" s="229"/>
+      <c r="G4" s="243"/>
+      <c r="H4" s="217"/>
+      <c r="I4" s="245"/>
+      <c r="J4" s="245"/>
+      <c r="K4" s="242"/>
+      <c r="L4" s="247"/>
       <c r="M4" s="156">
         <v>1</v>
       </c>
@@ -48500,337 +48499,337 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="227" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
-      <c r="G1" s="225"/>
-      <c r="H1" s="225"/>
-      <c r="I1" s="225"/>
-      <c r="J1" s="225"/>
-      <c r="K1" s="225"/>
-      <c r="L1" s="225"/>
-      <c r="M1" s="225"/>
-      <c r="N1" s="225"/>
-      <c r="O1" s="225"/>
-      <c r="P1" s="225"/>
-      <c r="Q1" s="225"/>
-      <c r="R1" s="225"/>
-      <c r="S1" s="225"/>
-      <c r="T1" s="225"/>
-      <c r="U1" s="225"/>
-      <c r="V1" s="225"/>
-      <c r="W1" s="225"/>
-      <c r="X1" s="225"/>
-      <c r="Y1" s="225"/>
-      <c r="Z1" s="225"/>
-      <c r="AA1" s="225"/>
-      <c r="AB1" s="225"/>
-      <c r="AC1" s="225"/>
-      <c r="AD1" s="225"/>
-      <c r="AE1" s="225"/>
-      <c r="AF1" s="225"/>
-      <c r="AG1" s="225"/>
-      <c r="AH1" s="225"/>
-      <c r="AI1" s="225"/>
-      <c r="AJ1" s="225"/>
-      <c r="AK1" s="225"/>
-      <c r="AL1" s="225"/>
-      <c r="AM1" s="225"/>
-      <c r="AN1" s="225"/>
-      <c r="AO1" s="225"/>
-      <c r="AP1" s="225"/>
-      <c r="AQ1" s="225"/>
-      <c r="AR1" s="225"/>
-      <c r="AS1" s="225"/>
-      <c r="AT1" s="225"/>
-      <c r="AU1" s="225"/>
-      <c r="AV1" s="225"/>
-      <c r="AW1" s="225"/>
-      <c r="AX1" s="225"/>
-      <c r="AY1" s="225"/>
-      <c r="AZ1" s="225"/>
-      <c r="BA1" s="225"/>
-      <c r="BB1" s="225"/>
-      <c r="BC1" s="225"/>
-      <c r="BD1" s="225"/>
-      <c r="BE1" s="225"/>
-      <c r="BF1" s="225"/>
-      <c r="BG1" s="225"/>
-      <c r="BH1" s="225"/>
-      <c r="BI1" s="225"/>
-      <c r="BJ1" s="225"/>
-      <c r="BK1" s="225"/>
-      <c r="BL1" s="225"/>
-      <c r="BM1" s="225"/>
-      <c r="BN1" s="225"/>
-      <c r="BO1" s="225"/>
-      <c r="BP1" s="225"/>
-      <c r="BQ1" s="225"/>
-      <c r="BR1" s="225"/>
-      <c r="BS1" s="225"/>
-      <c r="BT1" s="225"/>
-      <c r="BU1" s="225"/>
-      <c r="BV1" s="225"/>
-      <c r="BW1" s="225"/>
-      <c r="BX1" s="225"/>
-      <c r="BY1" s="225"/>
-      <c r="BZ1" s="225"/>
-      <c r="CA1" s="225"/>
-      <c r="CB1" s="225"/>
-      <c r="CC1" s="225"/>
-      <c r="CD1" s="225"/>
-      <c r="CE1" s="225"/>
-      <c r="CF1" s="225"/>
-      <c r="CG1" s="225"/>
-      <c r="CH1" s="225"/>
-      <c r="CI1" s="225"/>
-      <c r="CJ1" s="225"/>
-      <c r="CK1" s="225"/>
-      <c r="CL1" s="225"/>
-      <c r="CM1" s="225"/>
-      <c r="CN1" s="225"/>
-      <c r="CO1" s="225"/>
-      <c r="CP1" s="225"/>
-      <c r="CQ1" s="225"/>
-      <c r="CR1" s="225"/>
-      <c r="CS1" s="225"/>
-      <c r="CT1" s="225"/>
-      <c r="CU1" s="225"/>
-      <c r="CV1" s="225"/>
-      <c r="CW1" s="225"/>
-      <c r="CX1" s="225"/>
-      <c r="CY1" s="225"/>
-      <c r="CZ1" s="225"/>
-      <c r="DA1" s="225"/>
-      <c r="DB1" s="225"/>
-      <c r="DC1" s="225"/>
-      <c r="DD1" s="225"/>
-      <c r="DE1" s="225"/>
-      <c r="DF1" s="225"/>
-      <c r="DG1" s="225"/>
-      <c r="DH1" s="225"/>
-      <c r="DI1" s="225"/>
-      <c r="DJ1" s="225"/>
-      <c r="DK1" s="225"/>
-      <c r="DL1" s="225"/>
-      <c r="DM1" s="225"/>
-      <c r="DN1" s="225"/>
-      <c r="DO1" s="225"/>
-      <c r="DP1" s="225"/>
-      <c r="DQ1" s="225"/>
-      <c r="DR1" s="225"/>
-      <c r="DS1" s="225"/>
-      <c r="DT1" s="225"/>
-      <c r="DU1" s="225"/>
-      <c r="DV1" s="225"/>
-      <c r="DW1" s="225"/>
-      <c r="DX1" s="225"/>
-      <c r="DY1" s="225"/>
-      <c r="DZ1" s="225"/>
-      <c r="EA1" s="225"/>
-      <c r="EB1" s="225"/>
-      <c r="EC1" s="225"/>
-      <c r="ED1" s="225"/>
-      <c r="EE1" s="225"/>
-      <c r="EF1" s="225"/>
-      <c r="EG1" s="225"/>
-      <c r="EH1" s="225"/>
-      <c r="EI1" s="225"/>
-      <c r="EJ1" s="225"/>
-      <c r="EK1" s="225"/>
-      <c r="EL1" s="225"/>
-      <c r="EM1" s="225"/>
-      <c r="EN1" s="225"/>
-      <c r="EO1" s="225"/>
-      <c r="EP1" s="225"/>
-      <c r="EQ1" s="225"/>
-      <c r="ER1" s="225"/>
-      <c r="ES1" s="225"/>
-      <c r="ET1" s="225"/>
-      <c r="EU1" s="225"/>
-      <c r="EV1" s="225"/>
-      <c r="EW1" s="225"/>
-      <c r="EX1" s="225"/>
-      <c r="EY1" s="225"/>
-      <c r="EZ1" s="225"/>
-      <c r="FA1" s="225"/>
-      <c r="FB1" s="225"/>
-      <c r="FC1" s="225"/>
-      <c r="FD1" s="225"/>
-      <c r="FE1" s="225"/>
-      <c r="FF1" s="225"/>
-      <c r="FG1" s="225"/>
-      <c r="FH1" s="225"/>
-      <c r="FI1" s="225"/>
-      <c r="FJ1" s="225"/>
-      <c r="FK1" s="225"/>
-      <c r="FL1" s="225"/>
-      <c r="FM1" s="225"/>
-      <c r="FN1" s="225"/>
-      <c r="FO1" s="225"/>
-      <c r="FP1" s="225"/>
-      <c r="FQ1" s="225"/>
-      <c r="FR1" s="225"/>
-      <c r="FS1" s="225"/>
-      <c r="FT1" s="225"/>
-      <c r="FU1" s="225"/>
-      <c r="FV1" s="225"/>
-      <c r="FW1" s="225"/>
-      <c r="FX1" s="225"/>
-      <c r="FY1" s="225"/>
-      <c r="FZ1" s="225"/>
-      <c r="GA1" s="225"/>
-      <c r="GB1" s="225"/>
-      <c r="GC1" s="225"/>
-      <c r="GD1" s="225"/>
-      <c r="GE1" s="225"/>
-      <c r="GF1" s="225"/>
-      <c r="GG1" s="225"/>
-      <c r="GH1" s="225"/>
-      <c r="GI1" s="225"/>
-      <c r="GJ1" s="225"/>
-      <c r="GK1" s="225"/>
-      <c r="GL1" s="225"/>
-      <c r="GM1" s="225"/>
-      <c r="GN1" s="225"/>
-      <c r="GO1" s="225"/>
-      <c r="GP1" s="225"/>
-      <c r="GQ1" s="225"/>
-      <c r="GR1" s="225"/>
-      <c r="GS1" s="225"/>
-      <c r="GT1" s="225"/>
-      <c r="GU1" s="225"/>
-      <c r="GV1" s="225"/>
-      <c r="GW1" s="225"/>
-      <c r="GX1" s="225"/>
-      <c r="GY1" s="225"/>
-      <c r="GZ1" s="225"/>
-      <c r="HA1" s="225"/>
-      <c r="HB1" s="225"/>
-      <c r="HC1" s="225"/>
-      <c r="HD1" s="225"/>
-      <c r="HE1" s="225"/>
-      <c r="HF1" s="225"/>
-      <c r="HG1" s="225"/>
-      <c r="HH1" s="225"/>
-      <c r="HI1" s="225"/>
-      <c r="HJ1" s="225"/>
-      <c r="HK1" s="225"/>
-      <c r="HL1" s="225"/>
-      <c r="HM1" s="225"/>
-      <c r="HN1" s="225"/>
-      <c r="HO1" s="225"/>
-      <c r="HP1" s="225"/>
-      <c r="HQ1" s="225"/>
-      <c r="HR1" s="225"/>
-      <c r="HS1" s="225"/>
-      <c r="HT1" s="225"/>
-      <c r="HU1" s="225"/>
-      <c r="HV1" s="225"/>
-      <c r="HW1" s="225"/>
-      <c r="HX1" s="225"/>
-      <c r="HY1" s="225"/>
-      <c r="HZ1" s="225"/>
-      <c r="IA1" s="225"/>
-      <c r="IB1" s="225"/>
-      <c r="IC1" s="225"/>
-      <c r="ID1" s="225"/>
-      <c r="IE1" s="225"/>
-      <c r="IF1" s="225"/>
-      <c r="IG1" s="225"/>
-      <c r="IH1" s="225"/>
-      <c r="II1" s="225"/>
-      <c r="IJ1" s="225"/>
-      <c r="IK1" s="225"/>
-      <c r="IL1" s="225"/>
-      <c r="IM1" s="225"/>
-      <c r="IN1" s="225"/>
-      <c r="IO1" s="225"/>
-      <c r="IP1" s="225"/>
-      <c r="IQ1" s="225"/>
-      <c r="IR1" s="225"/>
-      <c r="IS1" s="225"/>
-      <c r="IT1" s="225"/>
-      <c r="IU1" s="225"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+      <c r="H1" s="227"/>
+      <c r="I1" s="227"/>
+      <c r="J1" s="227"/>
+      <c r="K1" s="227"/>
+      <c r="L1" s="227"/>
+      <c r="M1" s="227"/>
+      <c r="N1" s="227"/>
+      <c r="O1" s="227"/>
+      <c r="P1" s="227"/>
+      <c r="Q1" s="227"/>
+      <c r="R1" s="227"/>
+      <c r="S1" s="227"/>
+      <c r="T1" s="227"/>
+      <c r="U1" s="227"/>
+      <c r="V1" s="227"/>
+      <c r="W1" s="227"/>
+      <c r="X1" s="227"/>
+      <c r="Y1" s="227"/>
+      <c r="Z1" s="227"/>
+      <c r="AA1" s="227"/>
+      <c r="AB1" s="227"/>
+      <c r="AC1" s="227"/>
+      <c r="AD1" s="227"/>
+      <c r="AE1" s="227"/>
+      <c r="AF1" s="227"/>
+      <c r="AG1" s="227"/>
+      <c r="AH1" s="227"/>
+      <c r="AI1" s="227"/>
+      <c r="AJ1" s="227"/>
+      <c r="AK1" s="227"/>
+      <c r="AL1" s="227"/>
+      <c r="AM1" s="227"/>
+      <c r="AN1" s="227"/>
+      <c r="AO1" s="227"/>
+      <c r="AP1" s="227"/>
+      <c r="AQ1" s="227"/>
+      <c r="AR1" s="227"/>
+      <c r="AS1" s="227"/>
+      <c r="AT1" s="227"/>
+      <c r="AU1" s="227"/>
+      <c r="AV1" s="227"/>
+      <c r="AW1" s="227"/>
+      <c r="AX1" s="227"/>
+      <c r="AY1" s="227"/>
+      <c r="AZ1" s="227"/>
+      <c r="BA1" s="227"/>
+      <c r="BB1" s="227"/>
+      <c r="BC1" s="227"/>
+      <c r="BD1" s="227"/>
+      <c r="BE1" s="227"/>
+      <c r="BF1" s="227"/>
+      <c r="BG1" s="227"/>
+      <c r="BH1" s="227"/>
+      <c r="BI1" s="227"/>
+      <c r="BJ1" s="227"/>
+      <c r="BK1" s="227"/>
+      <c r="BL1" s="227"/>
+      <c r="BM1" s="227"/>
+      <c r="BN1" s="227"/>
+      <c r="BO1" s="227"/>
+      <c r="BP1" s="227"/>
+      <c r="BQ1" s="227"/>
+      <c r="BR1" s="227"/>
+      <c r="BS1" s="227"/>
+      <c r="BT1" s="227"/>
+      <c r="BU1" s="227"/>
+      <c r="BV1" s="227"/>
+      <c r="BW1" s="227"/>
+      <c r="BX1" s="227"/>
+      <c r="BY1" s="227"/>
+      <c r="BZ1" s="227"/>
+      <c r="CA1" s="227"/>
+      <c r="CB1" s="227"/>
+      <c r="CC1" s="227"/>
+      <c r="CD1" s="227"/>
+      <c r="CE1" s="227"/>
+      <c r="CF1" s="227"/>
+      <c r="CG1" s="227"/>
+      <c r="CH1" s="227"/>
+      <c r="CI1" s="227"/>
+      <c r="CJ1" s="227"/>
+      <c r="CK1" s="227"/>
+      <c r="CL1" s="227"/>
+      <c r="CM1" s="227"/>
+      <c r="CN1" s="227"/>
+      <c r="CO1" s="227"/>
+      <c r="CP1" s="227"/>
+      <c r="CQ1" s="227"/>
+      <c r="CR1" s="227"/>
+      <c r="CS1" s="227"/>
+      <c r="CT1" s="227"/>
+      <c r="CU1" s="227"/>
+      <c r="CV1" s="227"/>
+      <c r="CW1" s="227"/>
+      <c r="CX1" s="227"/>
+      <c r="CY1" s="227"/>
+      <c r="CZ1" s="227"/>
+      <c r="DA1" s="227"/>
+      <c r="DB1" s="227"/>
+      <c r="DC1" s="227"/>
+      <c r="DD1" s="227"/>
+      <c r="DE1" s="227"/>
+      <c r="DF1" s="227"/>
+      <c r="DG1" s="227"/>
+      <c r="DH1" s="227"/>
+      <c r="DI1" s="227"/>
+      <c r="DJ1" s="227"/>
+      <c r="DK1" s="227"/>
+      <c r="DL1" s="227"/>
+      <c r="DM1" s="227"/>
+      <c r="DN1" s="227"/>
+      <c r="DO1" s="227"/>
+      <c r="DP1" s="227"/>
+      <c r="DQ1" s="227"/>
+      <c r="DR1" s="227"/>
+      <c r="DS1" s="227"/>
+      <c r="DT1" s="227"/>
+      <c r="DU1" s="227"/>
+      <c r="DV1" s="227"/>
+      <c r="DW1" s="227"/>
+      <c r="DX1" s="227"/>
+      <c r="DY1" s="227"/>
+      <c r="DZ1" s="227"/>
+      <c r="EA1" s="227"/>
+      <c r="EB1" s="227"/>
+      <c r="EC1" s="227"/>
+      <c r="ED1" s="227"/>
+      <c r="EE1" s="227"/>
+      <c r="EF1" s="227"/>
+      <c r="EG1" s="227"/>
+      <c r="EH1" s="227"/>
+      <c r="EI1" s="227"/>
+      <c r="EJ1" s="227"/>
+      <c r="EK1" s="227"/>
+      <c r="EL1" s="227"/>
+      <c r="EM1" s="227"/>
+      <c r="EN1" s="227"/>
+      <c r="EO1" s="227"/>
+      <c r="EP1" s="227"/>
+      <c r="EQ1" s="227"/>
+      <c r="ER1" s="227"/>
+      <c r="ES1" s="227"/>
+      <c r="ET1" s="227"/>
+      <c r="EU1" s="227"/>
+      <c r="EV1" s="227"/>
+      <c r="EW1" s="227"/>
+      <c r="EX1" s="227"/>
+      <c r="EY1" s="227"/>
+      <c r="EZ1" s="227"/>
+      <c r="FA1" s="227"/>
+      <c r="FB1" s="227"/>
+      <c r="FC1" s="227"/>
+      <c r="FD1" s="227"/>
+      <c r="FE1" s="227"/>
+      <c r="FF1" s="227"/>
+      <c r="FG1" s="227"/>
+      <c r="FH1" s="227"/>
+      <c r="FI1" s="227"/>
+      <c r="FJ1" s="227"/>
+      <c r="FK1" s="227"/>
+      <c r="FL1" s="227"/>
+      <c r="FM1" s="227"/>
+      <c r="FN1" s="227"/>
+      <c r="FO1" s="227"/>
+      <c r="FP1" s="227"/>
+      <c r="FQ1" s="227"/>
+      <c r="FR1" s="227"/>
+      <c r="FS1" s="227"/>
+      <c r="FT1" s="227"/>
+      <c r="FU1" s="227"/>
+      <c r="FV1" s="227"/>
+      <c r="FW1" s="227"/>
+      <c r="FX1" s="227"/>
+      <c r="FY1" s="227"/>
+      <c r="FZ1" s="227"/>
+      <c r="GA1" s="227"/>
+      <c r="GB1" s="227"/>
+      <c r="GC1" s="227"/>
+      <c r="GD1" s="227"/>
+      <c r="GE1" s="227"/>
+      <c r="GF1" s="227"/>
+      <c r="GG1" s="227"/>
+      <c r="GH1" s="227"/>
+      <c r="GI1" s="227"/>
+      <c r="GJ1" s="227"/>
+      <c r="GK1" s="227"/>
+      <c r="GL1" s="227"/>
+      <c r="GM1" s="227"/>
+      <c r="GN1" s="227"/>
+      <c r="GO1" s="227"/>
+      <c r="GP1" s="227"/>
+      <c r="GQ1" s="227"/>
+      <c r="GR1" s="227"/>
+      <c r="GS1" s="227"/>
+      <c r="GT1" s="227"/>
+      <c r="GU1" s="227"/>
+      <c r="GV1" s="227"/>
+      <c r="GW1" s="227"/>
+      <c r="GX1" s="227"/>
+      <c r="GY1" s="227"/>
+      <c r="GZ1" s="227"/>
+      <c r="HA1" s="227"/>
+      <c r="HB1" s="227"/>
+      <c r="HC1" s="227"/>
+      <c r="HD1" s="227"/>
+      <c r="HE1" s="227"/>
+      <c r="HF1" s="227"/>
+      <c r="HG1" s="227"/>
+      <c r="HH1" s="227"/>
+      <c r="HI1" s="227"/>
+      <c r="HJ1" s="227"/>
+      <c r="HK1" s="227"/>
+      <c r="HL1" s="227"/>
+      <c r="HM1" s="227"/>
+      <c r="HN1" s="227"/>
+      <c r="HO1" s="227"/>
+      <c r="HP1" s="227"/>
+      <c r="HQ1" s="227"/>
+      <c r="HR1" s="227"/>
+      <c r="HS1" s="227"/>
+      <c r="HT1" s="227"/>
+      <c r="HU1" s="227"/>
+      <c r="HV1" s="227"/>
+      <c r="HW1" s="227"/>
+      <c r="HX1" s="227"/>
+      <c r="HY1" s="227"/>
+      <c r="HZ1" s="227"/>
+      <c r="IA1" s="227"/>
+      <c r="IB1" s="227"/>
+      <c r="IC1" s="227"/>
+      <c r="ID1" s="227"/>
+      <c r="IE1" s="227"/>
+      <c r="IF1" s="227"/>
+      <c r="IG1" s="227"/>
+      <c r="IH1" s="227"/>
+      <c r="II1" s="227"/>
+      <c r="IJ1" s="227"/>
+      <c r="IK1" s="227"/>
+      <c r="IL1" s="227"/>
+      <c r="IM1" s="227"/>
+      <c r="IN1" s="227"/>
+      <c r="IO1" s="227"/>
+      <c r="IP1" s="227"/>
+      <c r="IQ1" s="227"/>
+      <c r="IR1" s="227"/>
+      <c r="IS1" s="227"/>
+      <c r="IT1" s="227"/>
+      <c r="IU1" s="227"/>
     </row>
     <row r="2" spans="1:255" ht="15.75" thickBot="1">
-      <c r="A2" s="228" t="str">
+      <c r="A2" s="230" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
     </row>
     <row r="3" spans="1:255" ht="15" customHeight="1">
-      <c r="A3" s="229" t="str">
+      <c r="A3" s="231" t="str">
         <f>'Сводная таблица'!A3:A4</f>
         <v>№ п/п</v>
       </c>
-      <c r="B3" s="231" t="str">
+      <c r="B3" s="233" t="str">
         <f>'Сводная таблица'!B3:B4</f>
         <v>группа</v>
       </c>
-      <c r="C3" s="233" t="str">
+      <c r="C3" s="235" t="str">
         <f>'Сводная таблица'!C3:C4</f>
         <v>подргуппа</v>
       </c>
-      <c r="D3" s="235" t="str">
+      <c r="D3" s="237" t="str">
         <f>'Сводная таблица'!D3:D4</f>
         <v>Фамилия</v>
       </c>
-      <c r="E3" s="237" t="str">
+      <c r="E3" s="239" t="str">
         <f>'Сводная таблица'!E3:E4</f>
         <v>Имя</v>
       </c>
-      <c r="F3" s="226" t="str">
+      <c r="F3" s="228" t="str">
         <f>'Сводная таблица'!F3:F4</f>
         <v>Отчество</v>
       </c>
-      <c r="G3" s="229" t="s">
+      <c r="G3" s="231" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="235" t="s">
+      <c r="H3" s="237" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="242" t="s">
+      <c r="I3" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="242" t="s">
+      <c r="J3" s="244" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="247" t="s">
+      <c r="K3" s="249" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="249" t="s">
+      <c r="L3" s="251" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:255" ht="15.75" thickBot="1">
-      <c r="A4" s="230"/>
-      <c r="B4" s="232"/>
-      <c r="C4" s="234"/>
-      <c r="D4" s="236"/>
-      <c r="E4" s="238"/>
-      <c r="F4" s="227"/>
-      <c r="G4" s="241"/>
-      <c r="H4" s="236"/>
-      <c r="I4" s="246"/>
-      <c r="J4" s="246"/>
-      <c r="K4" s="248"/>
-      <c r="L4" s="250"/>
+      <c r="A4" s="232"/>
+      <c r="B4" s="234"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="238"/>
+      <c r="E4" s="240"/>
+      <c r="F4" s="229"/>
+      <c r="G4" s="243"/>
+      <c r="H4" s="238"/>
+      <c r="I4" s="248"/>
+      <c r="J4" s="248"/>
+      <c r="K4" s="250"/>
+      <c r="L4" s="252"/>
     </row>
     <row r="5" spans="1:255" s="40" customFormat="1">
       <c r="A5" s="145">
@@ -50565,338 +50564,338 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="227" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
-      <c r="G1" s="225"/>
-      <c r="H1" s="225"/>
-      <c r="I1" s="225"/>
-      <c r="J1" s="225"/>
-      <c r="K1" s="225"/>
-      <c r="L1" s="225"/>
-      <c r="M1" s="225"/>
-      <c r="N1" s="225"/>
-      <c r="O1" s="225"/>
-      <c r="P1" s="225"/>
-      <c r="Q1" s="225"/>
-      <c r="R1" s="225"/>
-      <c r="S1" s="225"/>
-      <c r="T1" s="225"/>
-      <c r="U1" s="225"/>
-      <c r="V1" s="225"/>
-      <c r="W1" s="225"/>
-      <c r="X1" s="225"/>
-      <c r="Y1" s="225"/>
-      <c r="Z1" s="225"/>
-      <c r="AA1" s="225"/>
-      <c r="AB1" s="225"/>
-      <c r="AC1" s="225"/>
-      <c r="AD1" s="225"/>
-      <c r="AE1" s="225"/>
-      <c r="AF1" s="225"/>
-      <c r="AG1" s="225"/>
-      <c r="AH1" s="225"/>
-      <c r="AI1" s="225"/>
-      <c r="AJ1" s="225"/>
-      <c r="AK1" s="225"/>
-      <c r="AL1" s="225"/>
-      <c r="AM1" s="225"/>
-      <c r="AN1" s="225"/>
-      <c r="AO1" s="225"/>
-      <c r="AP1" s="225"/>
-      <c r="AQ1" s="225"/>
-      <c r="AR1" s="225"/>
-      <c r="AS1" s="225"/>
-      <c r="AT1" s="225"/>
-      <c r="AU1" s="225"/>
-      <c r="AV1" s="225"/>
-      <c r="AW1" s="225"/>
-      <c r="AX1" s="225"/>
-      <c r="AY1" s="225"/>
-      <c r="AZ1" s="225"/>
-      <c r="BA1" s="225"/>
-      <c r="BB1" s="225"/>
-      <c r="BC1" s="225"/>
-      <c r="BD1" s="225"/>
-      <c r="BE1" s="225"/>
-      <c r="BF1" s="225"/>
-      <c r="BG1" s="225"/>
-      <c r="BH1" s="225"/>
-      <c r="BI1" s="225"/>
-      <c r="BJ1" s="225"/>
-      <c r="BK1" s="225"/>
-      <c r="BL1" s="225"/>
-      <c r="BM1" s="225"/>
-      <c r="BN1" s="225"/>
-      <c r="BO1" s="225"/>
-      <c r="BP1" s="225"/>
-      <c r="BQ1" s="225"/>
-      <c r="BR1" s="225"/>
-      <c r="BS1" s="225"/>
-      <c r="BT1" s="225"/>
-      <c r="BU1" s="225"/>
-      <c r="BV1" s="225"/>
-      <c r="BW1" s="225"/>
-      <c r="BX1" s="225"/>
-      <c r="BY1" s="225"/>
-      <c r="BZ1" s="225"/>
-      <c r="CA1" s="225"/>
-      <c r="CB1" s="225"/>
-      <c r="CC1" s="225"/>
-      <c r="CD1" s="225"/>
-      <c r="CE1" s="225"/>
-      <c r="CF1" s="225"/>
-      <c r="CG1" s="225"/>
-      <c r="CH1" s="225"/>
-      <c r="CI1" s="225"/>
-      <c r="CJ1" s="225"/>
-      <c r="CK1" s="225"/>
-      <c r="CL1" s="225"/>
-      <c r="CM1" s="225"/>
-      <c r="CN1" s="225"/>
-      <c r="CO1" s="225"/>
-      <c r="CP1" s="225"/>
-      <c r="CQ1" s="225"/>
-      <c r="CR1" s="225"/>
-      <c r="CS1" s="225"/>
-      <c r="CT1" s="225"/>
-      <c r="CU1" s="225"/>
-      <c r="CV1" s="225"/>
-      <c r="CW1" s="225"/>
-      <c r="CX1" s="225"/>
-      <c r="CY1" s="225"/>
-      <c r="CZ1" s="225"/>
-      <c r="DA1" s="225"/>
-      <c r="DB1" s="225"/>
-      <c r="DC1" s="225"/>
-      <c r="DD1" s="225"/>
-      <c r="DE1" s="225"/>
-      <c r="DF1" s="225"/>
-      <c r="DG1" s="225"/>
-      <c r="DH1" s="225"/>
-      <c r="DI1" s="225"/>
-      <c r="DJ1" s="225"/>
-      <c r="DK1" s="225"/>
-      <c r="DL1" s="225"/>
-      <c r="DM1" s="225"/>
-      <c r="DN1" s="225"/>
-      <c r="DO1" s="225"/>
-      <c r="DP1" s="225"/>
-      <c r="DQ1" s="225"/>
-      <c r="DR1" s="225"/>
-      <c r="DS1" s="225"/>
-      <c r="DT1" s="225"/>
-      <c r="DU1" s="225"/>
-      <c r="DV1" s="225"/>
-      <c r="DW1" s="225"/>
-      <c r="DX1" s="225"/>
-      <c r="DY1" s="225"/>
-      <c r="DZ1" s="225"/>
-      <c r="EA1" s="225"/>
-      <c r="EB1" s="225"/>
-      <c r="EC1" s="225"/>
-      <c r="ED1" s="225"/>
-      <c r="EE1" s="225"/>
-      <c r="EF1" s="225"/>
-      <c r="EG1" s="225"/>
-      <c r="EH1" s="225"/>
-      <c r="EI1" s="225"/>
-      <c r="EJ1" s="225"/>
-      <c r="EK1" s="225"/>
-      <c r="EL1" s="225"/>
-      <c r="EM1" s="225"/>
-      <c r="EN1" s="225"/>
-      <c r="EO1" s="225"/>
-      <c r="EP1" s="225"/>
-      <c r="EQ1" s="225"/>
-      <c r="ER1" s="225"/>
-      <c r="ES1" s="225"/>
-      <c r="ET1" s="225"/>
-      <c r="EU1" s="225"/>
-      <c r="EV1" s="225"/>
-      <c r="EW1" s="225"/>
-      <c r="EX1" s="225"/>
-      <c r="EY1" s="225"/>
-      <c r="EZ1" s="225"/>
-      <c r="FA1" s="225"/>
-      <c r="FB1" s="225"/>
-      <c r="FC1" s="225"/>
-      <c r="FD1" s="225"/>
-      <c r="FE1" s="225"/>
-      <c r="FF1" s="225"/>
-      <c r="FG1" s="225"/>
-      <c r="FH1" s="225"/>
-      <c r="FI1" s="225"/>
-      <c r="FJ1" s="225"/>
-      <c r="FK1" s="225"/>
-      <c r="FL1" s="225"/>
-      <c r="FM1" s="225"/>
-      <c r="FN1" s="225"/>
-      <c r="FO1" s="225"/>
-      <c r="FP1" s="225"/>
-      <c r="FQ1" s="225"/>
-      <c r="FR1" s="225"/>
-      <c r="FS1" s="225"/>
-      <c r="FT1" s="225"/>
-      <c r="FU1" s="225"/>
-      <c r="FV1" s="225"/>
-      <c r="FW1" s="225"/>
-      <c r="FX1" s="225"/>
-      <c r="FY1" s="225"/>
-      <c r="FZ1" s="225"/>
-      <c r="GA1" s="225"/>
-      <c r="GB1" s="225"/>
-      <c r="GC1" s="225"/>
-      <c r="GD1" s="225"/>
-      <c r="GE1" s="225"/>
-      <c r="GF1" s="225"/>
-      <c r="GG1" s="225"/>
-      <c r="GH1" s="225"/>
-      <c r="GI1" s="225"/>
-      <c r="GJ1" s="225"/>
-      <c r="GK1" s="225"/>
-      <c r="GL1" s="225"/>
-      <c r="GM1" s="225"/>
-      <c r="GN1" s="225"/>
-      <c r="GO1" s="225"/>
-      <c r="GP1" s="225"/>
-      <c r="GQ1" s="225"/>
-      <c r="GR1" s="225"/>
-      <c r="GS1" s="225"/>
-      <c r="GT1" s="225"/>
-      <c r="GU1" s="225"/>
-      <c r="GV1" s="225"/>
-      <c r="GW1" s="225"/>
-      <c r="GX1" s="225"/>
-      <c r="GY1" s="225"/>
-      <c r="GZ1" s="225"/>
-      <c r="HA1" s="225"/>
-      <c r="HB1" s="225"/>
-      <c r="HC1" s="225"/>
-      <c r="HD1" s="225"/>
-      <c r="HE1" s="225"/>
-      <c r="HF1" s="225"/>
-      <c r="HG1" s="225"/>
-      <c r="HH1" s="225"/>
-      <c r="HI1" s="225"/>
-      <c r="HJ1" s="225"/>
-      <c r="HK1" s="225"/>
-      <c r="HL1" s="225"/>
-      <c r="HM1" s="225"/>
-      <c r="HN1" s="225"/>
-      <c r="HO1" s="225"/>
-      <c r="HP1" s="225"/>
-      <c r="HQ1" s="225"/>
-      <c r="HR1" s="225"/>
-      <c r="HS1" s="225"/>
-      <c r="HT1" s="225"/>
-      <c r="HU1" s="225"/>
-      <c r="HV1" s="225"/>
-      <c r="HW1" s="225"/>
-      <c r="HX1" s="225"/>
-      <c r="HY1" s="225"/>
-      <c r="HZ1" s="225"/>
-      <c r="IA1" s="225"/>
-      <c r="IB1" s="225"/>
-      <c r="IC1" s="225"/>
-      <c r="ID1" s="225"/>
-      <c r="IE1" s="225"/>
-      <c r="IF1" s="225"/>
-      <c r="IG1" s="225"/>
-      <c r="IH1" s="225"/>
-      <c r="II1" s="225"/>
-      <c r="IJ1" s="225"/>
-      <c r="IK1" s="225"/>
-      <c r="IL1" s="225"/>
-      <c r="IM1" s="225"/>
-      <c r="IN1" s="225"/>
-      <c r="IO1" s="225"/>
-      <c r="IP1" s="225"/>
-      <c r="IQ1" s="225"/>
-      <c r="IR1" s="225"/>
-      <c r="IS1" s="225"/>
-      <c r="IT1" s="225"/>
-      <c r="IU1" s="225"/>
-      <c r="IV1" s="225"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+      <c r="H1" s="227"/>
+      <c r="I1" s="227"/>
+      <c r="J1" s="227"/>
+      <c r="K1" s="227"/>
+      <c r="L1" s="227"/>
+      <c r="M1" s="227"/>
+      <c r="N1" s="227"/>
+      <c r="O1" s="227"/>
+      <c r="P1" s="227"/>
+      <c r="Q1" s="227"/>
+      <c r="R1" s="227"/>
+      <c r="S1" s="227"/>
+      <c r="T1" s="227"/>
+      <c r="U1" s="227"/>
+      <c r="V1" s="227"/>
+      <c r="W1" s="227"/>
+      <c r="X1" s="227"/>
+      <c r="Y1" s="227"/>
+      <c r="Z1" s="227"/>
+      <c r="AA1" s="227"/>
+      <c r="AB1" s="227"/>
+      <c r="AC1" s="227"/>
+      <c r="AD1" s="227"/>
+      <c r="AE1" s="227"/>
+      <c r="AF1" s="227"/>
+      <c r="AG1" s="227"/>
+      <c r="AH1" s="227"/>
+      <c r="AI1" s="227"/>
+      <c r="AJ1" s="227"/>
+      <c r="AK1" s="227"/>
+      <c r="AL1" s="227"/>
+      <c r="AM1" s="227"/>
+      <c r="AN1" s="227"/>
+      <c r="AO1" s="227"/>
+      <c r="AP1" s="227"/>
+      <c r="AQ1" s="227"/>
+      <c r="AR1" s="227"/>
+      <c r="AS1" s="227"/>
+      <c r="AT1" s="227"/>
+      <c r="AU1" s="227"/>
+      <c r="AV1" s="227"/>
+      <c r="AW1" s="227"/>
+      <c r="AX1" s="227"/>
+      <c r="AY1" s="227"/>
+      <c r="AZ1" s="227"/>
+      <c r="BA1" s="227"/>
+      <c r="BB1" s="227"/>
+      <c r="BC1" s="227"/>
+      <c r="BD1" s="227"/>
+      <c r="BE1" s="227"/>
+      <c r="BF1" s="227"/>
+      <c r="BG1" s="227"/>
+      <c r="BH1" s="227"/>
+      <c r="BI1" s="227"/>
+      <c r="BJ1" s="227"/>
+      <c r="BK1" s="227"/>
+      <c r="BL1" s="227"/>
+      <c r="BM1" s="227"/>
+      <c r="BN1" s="227"/>
+      <c r="BO1" s="227"/>
+      <c r="BP1" s="227"/>
+      <c r="BQ1" s="227"/>
+      <c r="BR1" s="227"/>
+      <c r="BS1" s="227"/>
+      <c r="BT1" s="227"/>
+      <c r="BU1" s="227"/>
+      <c r="BV1" s="227"/>
+      <c r="BW1" s="227"/>
+      <c r="BX1" s="227"/>
+      <c r="BY1" s="227"/>
+      <c r="BZ1" s="227"/>
+      <c r="CA1" s="227"/>
+      <c r="CB1" s="227"/>
+      <c r="CC1" s="227"/>
+      <c r="CD1" s="227"/>
+      <c r="CE1" s="227"/>
+      <c r="CF1" s="227"/>
+      <c r="CG1" s="227"/>
+      <c r="CH1" s="227"/>
+      <c r="CI1" s="227"/>
+      <c r="CJ1" s="227"/>
+      <c r="CK1" s="227"/>
+      <c r="CL1" s="227"/>
+      <c r="CM1" s="227"/>
+      <c r="CN1" s="227"/>
+      <c r="CO1" s="227"/>
+      <c r="CP1" s="227"/>
+      <c r="CQ1" s="227"/>
+      <c r="CR1" s="227"/>
+      <c r="CS1" s="227"/>
+      <c r="CT1" s="227"/>
+      <c r="CU1" s="227"/>
+      <c r="CV1" s="227"/>
+      <c r="CW1" s="227"/>
+      <c r="CX1" s="227"/>
+      <c r="CY1" s="227"/>
+      <c r="CZ1" s="227"/>
+      <c r="DA1" s="227"/>
+      <c r="DB1" s="227"/>
+      <c r="DC1" s="227"/>
+      <c r="DD1" s="227"/>
+      <c r="DE1" s="227"/>
+      <c r="DF1" s="227"/>
+      <c r="DG1" s="227"/>
+      <c r="DH1" s="227"/>
+      <c r="DI1" s="227"/>
+      <c r="DJ1" s="227"/>
+      <c r="DK1" s="227"/>
+      <c r="DL1" s="227"/>
+      <c r="DM1" s="227"/>
+      <c r="DN1" s="227"/>
+      <c r="DO1" s="227"/>
+      <c r="DP1" s="227"/>
+      <c r="DQ1" s="227"/>
+      <c r="DR1" s="227"/>
+      <c r="DS1" s="227"/>
+      <c r="DT1" s="227"/>
+      <c r="DU1" s="227"/>
+      <c r="DV1" s="227"/>
+      <c r="DW1" s="227"/>
+      <c r="DX1" s="227"/>
+      <c r="DY1" s="227"/>
+      <c r="DZ1" s="227"/>
+      <c r="EA1" s="227"/>
+      <c r="EB1" s="227"/>
+      <c r="EC1" s="227"/>
+      <c r="ED1" s="227"/>
+      <c r="EE1" s="227"/>
+      <c r="EF1" s="227"/>
+      <c r="EG1" s="227"/>
+      <c r="EH1" s="227"/>
+      <c r="EI1" s="227"/>
+      <c r="EJ1" s="227"/>
+      <c r="EK1" s="227"/>
+      <c r="EL1" s="227"/>
+      <c r="EM1" s="227"/>
+      <c r="EN1" s="227"/>
+      <c r="EO1" s="227"/>
+      <c r="EP1" s="227"/>
+      <c r="EQ1" s="227"/>
+      <c r="ER1" s="227"/>
+      <c r="ES1" s="227"/>
+      <c r="ET1" s="227"/>
+      <c r="EU1" s="227"/>
+      <c r="EV1" s="227"/>
+      <c r="EW1" s="227"/>
+      <c r="EX1" s="227"/>
+      <c r="EY1" s="227"/>
+      <c r="EZ1" s="227"/>
+      <c r="FA1" s="227"/>
+      <c r="FB1" s="227"/>
+      <c r="FC1" s="227"/>
+      <c r="FD1" s="227"/>
+      <c r="FE1" s="227"/>
+      <c r="FF1" s="227"/>
+      <c r="FG1" s="227"/>
+      <c r="FH1" s="227"/>
+      <c r="FI1" s="227"/>
+      <c r="FJ1" s="227"/>
+      <c r="FK1" s="227"/>
+      <c r="FL1" s="227"/>
+      <c r="FM1" s="227"/>
+      <c r="FN1" s="227"/>
+      <c r="FO1" s="227"/>
+      <c r="FP1" s="227"/>
+      <c r="FQ1" s="227"/>
+      <c r="FR1" s="227"/>
+      <c r="FS1" s="227"/>
+      <c r="FT1" s="227"/>
+      <c r="FU1" s="227"/>
+      <c r="FV1" s="227"/>
+      <c r="FW1" s="227"/>
+      <c r="FX1" s="227"/>
+      <c r="FY1" s="227"/>
+      <c r="FZ1" s="227"/>
+      <c r="GA1" s="227"/>
+      <c r="GB1" s="227"/>
+      <c r="GC1" s="227"/>
+      <c r="GD1" s="227"/>
+      <c r="GE1" s="227"/>
+      <c r="GF1" s="227"/>
+      <c r="GG1" s="227"/>
+      <c r="GH1" s="227"/>
+      <c r="GI1" s="227"/>
+      <c r="GJ1" s="227"/>
+      <c r="GK1" s="227"/>
+      <c r="GL1" s="227"/>
+      <c r="GM1" s="227"/>
+      <c r="GN1" s="227"/>
+      <c r="GO1" s="227"/>
+      <c r="GP1" s="227"/>
+      <c r="GQ1" s="227"/>
+      <c r="GR1" s="227"/>
+      <c r="GS1" s="227"/>
+      <c r="GT1" s="227"/>
+      <c r="GU1" s="227"/>
+      <c r="GV1" s="227"/>
+      <c r="GW1" s="227"/>
+      <c r="GX1" s="227"/>
+      <c r="GY1" s="227"/>
+      <c r="GZ1" s="227"/>
+      <c r="HA1" s="227"/>
+      <c r="HB1" s="227"/>
+      <c r="HC1" s="227"/>
+      <c r="HD1" s="227"/>
+      <c r="HE1" s="227"/>
+      <c r="HF1" s="227"/>
+      <c r="HG1" s="227"/>
+      <c r="HH1" s="227"/>
+      <c r="HI1" s="227"/>
+      <c r="HJ1" s="227"/>
+      <c r="HK1" s="227"/>
+      <c r="HL1" s="227"/>
+      <c r="HM1" s="227"/>
+      <c r="HN1" s="227"/>
+      <c r="HO1" s="227"/>
+      <c r="HP1" s="227"/>
+      <c r="HQ1" s="227"/>
+      <c r="HR1" s="227"/>
+      <c r="HS1" s="227"/>
+      <c r="HT1" s="227"/>
+      <c r="HU1" s="227"/>
+      <c r="HV1" s="227"/>
+      <c r="HW1" s="227"/>
+      <c r="HX1" s="227"/>
+      <c r="HY1" s="227"/>
+      <c r="HZ1" s="227"/>
+      <c r="IA1" s="227"/>
+      <c r="IB1" s="227"/>
+      <c r="IC1" s="227"/>
+      <c r="ID1" s="227"/>
+      <c r="IE1" s="227"/>
+      <c r="IF1" s="227"/>
+      <c r="IG1" s="227"/>
+      <c r="IH1" s="227"/>
+      <c r="II1" s="227"/>
+      <c r="IJ1" s="227"/>
+      <c r="IK1" s="227"/>
+      <c r="IL1" s="227"/>
+      <c r="IM1" s="227"/>
+      <c r="IN1" s="227"/>
+      <c r="IO1" s="227"/>
+      <c r="IP1" s="227"/>
+      <c r="IQ1" s="227"/>
+      <c r="IR1" s="227"/>
+      <c r="IS1" s="227"/>
+      <c r="IT1" s="227"/>
+      <c r="IU1" s="227"/>
+      <c r="IV1" s="227"/>
     </row>
     <row r="2" spans="1:256" ht="15.75" thickBot="1">
-      <c r="A2" s="228" t="str">
+      <c r="A2" s="230" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
     </row>
     <row r="3" spans="1:256" ht="15" customHeight="1">
-      <c r="A3" s="229" t="str">
+      <c r="A3" s="231" t="str">
         <f>'Сводная таблица'!A3:A4</f>
         <v>№ п/п</v>
       </c>
-      <c r="B3" s="231" t="str">
+      <c r="B3" s="233" t="str">
         <f>'Сводная таблица'!B3:B4</f>
         <v>группа</v>
       </c>
-      <c r="C3" s="233" t="str">
+      <c r="C3" s="235" t="str">
         <f>'Сводная таблица'!C3:C4</f>
         <v>подргуппа</v>
       </c>
-      <c r="D3" s="235" t="str">
+      <c r="D3" s="237" t="str">
         <f>'Сводная таблица'!D3:D4</f>
         <v>Фамилия</v>
       </c>
-      <c r="E3" s="237" t="str">
+      <c r="E3" s="239" t="str">
         <f>'Сводная таблица'!E3:E4</f>
         <v>Имя</v>
       </c>
-      <c r="F3" s="226" t="str">
+      <c r="F3" s="228" t="str">
         <f>'Сводная таблица'!F3:F4</f>
         <v>Отчество</v>
       </c>
-      <c r="G3" s="229" t="s">
+      <c r="G3" s="231" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="235" t="s">
+      <c r="H3" s="237" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="242" t="s">
+      <c r="I3" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="242" t="s">
+      <c r="J3" s="244" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="247" t="s">
+      <c r="K3" s="249" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="249" t="s">
+      <c r="L3" s="251" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:256" ht="15.75" thickBot="1">
-      <c r="A4" s="230"/>
-      <c r="B4" s="232"/>
-      <c r="C4" s="234"/>
-      <c r="D4" s="236"/>
-      <c r="E4" s="238"/>
-      <c r="F4" s="227"/>
-      <c r="G4" s="230"/>
-      <c r="H4" s="236"/>
-      <c r="I4" s="246"/>
-      <c r="J4" s="246"/>
-      <c r="K4" s="248"/>
-      <c r="L4" s="250"/>
+      <c r="A4" s="232"/>
+      <c r="B4" s="234"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="238"/>
+      <c r="E4" s="240"/>
+      <c r="F4" s="229"/>
+      <c r="G4" s="232"/>
+      <c r="H4" s="238"/>
+      <c r="I4" s="248"/>
+      <c r="J4" s="248"/>
+      <c r="K4" s="250"/>
+      <c r="L4" s="252"/>
     </row>
     <row r="5" spans="1:256" s="40" customFormat="1">
       <c r="A5" s="145">
@@ -52583,337 +52582,337 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:255" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="227" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
-      <c r="G1" s="225"/>
-      <c r="H1" s="225"/>
-      <c r="I1" s="225"/>
-      <c r="J1" s="225"/>
-      <c r="K1" s="225"/>
-      <c r="L1" s="225"/>
-      <c r="M1" s="225"/>
-      <c r="N1" s="225"/>
-      <c r="O1" s="225"/>
-      <c r="P1" s="225"/>
-      <c r="Q1" s="225"/>
-      <c r="R1" s="225"/>
-      <c r="S1" s="225"/>
-      <c r="T1" s="225"/>
-      <c r="U1" s="225"/>
-      <c r="V1" s="225"/>
-      <c r="W1" s="225"/>
-      <c r="X1" s="225"/>
-      <c r="Y1" s="225"/>
-      <c r="Z1" s="225"/>
-      <c r="AA1" s="225"/>
-      <c r="AB1" s="225"/>
-      <c r="AC1" s="225"/>
-      <c r="AD1" s="225"/>
-      <c r="AE1" s="225"/>
-      <c r="AF1" s="225"/>
-      <c r="AG1" s="225"/>
-      <c r="AH1" s="225"/>
-      <c r="AI1" s="225"/>
-      <c r="AJ1" s="225"/>
-      <c r="AK1" s="225"/>
-      <c r="AL1" s="225"/>
-      <c r="AM1" s="225"/>
-      <c r="AN1" s="225"/>
-      <c r="AO1" s="225"/>
-      <c r="AP1" s="225"/>
-      <c r="AQ1" s="225"/>
-      <c r="AR1" s="225"/>
-      <c r="AS1" s="225"/>
-      <c r="AT1" s="225"/>
-      <c r="AU1" s="225"/>
-      <c r="AV1" s="225"/>
-      <c r="AW1" s="225"/>
-      <c r="AX1" s="225"/>
-      <c r="AY1" s="225"/>
-      <c r="AZ1" s="225"/>
-      <c r="BA1" s="225"/>
-      <c r="BB1" s="225"/>
-      <c r="BC1" s="225"/>
-      <c r="BD1" s="225"/>
-      <c r="BE1" s="225"/>
-      <c r="BF1" s="225"/>
-      <c r="BG1" s="225"/>
-      <c r="BH1" s="225"/>
-      <c r="BI1" s="225"/>
-      <c r="BJ1" s="225"/>
-      <c r="BK1" s="225"/>
-      <c r="BL1" s="225"/>
-      <c r="BM1" s="225"/>
-      <c r="BN1" s="225"/>
-      <c r="BO1" s="225"/>
-      <c r="BP1" s="225"/>
-      <c r="BQ1" s="225"/>
-      <c r="BR1" s="225"/>
-      <c r="BS1" s="225"/>
-      <c r="BT1" s="225"/>
-      <c r="BU1" s="225"/>
-      <c r="BV1" s="225"/>
-      <c r="BW1" s="225"/>
-      <c r="BX1" s="225"/>
-      <c r="BY1" s="225"/>
-      <c r="BZ1" s="225"/>
-      <c r="CA1" s="225"/>
-      <c r="CB1" s="225"/>
-      <c r="CC1" s="225"/>
-      <c r="CD1" s="225"/>
-      <c r="CE1" s="225"/>
-      <c r="CF1" s="225"/>
-      <c r="CG1" s="225"/>
-      <c r="CH1" s="225"/>
-      <c r="CI1" s="225"/>
-      <c r="CJ1" s="225"/>
-      <c r="CK1" s="225"/>
-      <c r="CL1" s="225"/>
-      <c r="CM1" s="225"/>
-      <c r="CN1" s="225"/>
-      <c r="CO1" s="225"/>
-      <c r="CP1" s="225"/>
-      <c r="CQ1" s="225"/>
-      <c r="CR1" s="225"/>
-      <c r="CS1" s="225"/>
-      <c r="CT1" s="225"/>
-      <c r="CU1" s="225"/>
-      <c r="CV1" s="225"/>
-      <c r="CW1" s="225"/>
-      <c r="CX1" s="225"/>
-      <c r="CY1" s="225"/>
-      <c r="CZ1" s="225"/>
-      <c r="DA1" s="225"/>
-      <c r="DB1" s="225"/>
-      <c r="DC1" s="225"/>
-      <c r="DD1" s="225"/>
-      <c r="DE1" s="225"/>
-      <c r="DF1" s="225"/>
-      <c r="DG1" s="225"/>
-      <c r="DH1" s="225"/>
-      <c r="DI1" s="225"/>
-      <c r="DJ1" s="225"/>
-      <c r="DK1" s="225"/>
-      <c r="DL1" s="225"/>
-      <c r="DM1" s="225"/>
-      <c r="DN1" s="225"/>
-      <c r="DO1" s="225"/>
-      <c r="DP1" s="225"/>
-      <c r="DQ1" s="225"/>
-      <c r="DR1" s="225"/>
-      <c r="DS1" s="225"/>
-      <c r="DT1" s="225"/>
-      <c r="DU1" s="225"/>
-      <c r="DV1" s="225"/>
-      <c r="DW1" s="225"/>
-      <c r="DX1" s="225"/>
-      <c r="DY1" s="225"/>
-      <c r="DZ1" s="225"/>
-      <c r="EA1" s="225"/>
-      <c r="EB1" s="225"/>
-      <c r="EC1" s="225"/>
-      <c r="ED1" s="225"/>
-      <c r="EE1" s="225"/>
-      <c r="EF1" s="225"/>
-      <c r="EG1" s="225"/>
-      <c r="EH1" s="225"/>
-      <c r="EI1" s="225"/>
-      <c r="EJ1" s="225"/>
-      <c r="EK1" s="225"/>
-      <c r="EL1" s="225"/>
-      <c r="EM1" s="225"/>
-      <c r="EN1" s="225"/>
-      <c r="EO1" s="225"/>
-      <c r="EP1" s="225"/>
-      <c r="EQ1" s="225"/>
-      <c r="ER1" s="225"/>
-      <c r="ES1" s="225"/>
-      <c r="ET1" s="225"/>
-      <c r="EU1" s="225"/>
-      <c r="EV1" s="225"/>
-      <c r="EW1" s="225"/>
-      <c r="EX1" s="225"/>
-      <c r="EY1" s="225"/>
-      <c r="EZ1" s="225"/>
-      <c r="FA1" s="225"/>
-      <c r="FB1" s="225"/>
-      <c r="FC1" s="225"/>
-      <c r="FD1" s="225"/>
-      <c r="FE1" s="225"/>
-      <c r="FF1" s="225"/>
-      <c r="FG1" s="225"/>
-      <c r="FH1" s="225"/>
-      <c r="FI1" s="225"/>
-      <c r="FJ1" s="225"/>
-      <c r="FK1" s="225"/>
-      <c r="FL1" s="225"/>
-      <c r="FM1" s="225"/>
-      <c r="FN1" s="225"/>
-      <c r="FO1" s="225"/>
-      <c r="FP1" s="225"/>
-      <c r="FQ1" s="225"/>
-      <c r="FR1" s="225"/>
-      <c r="FS1" s="225"/>
-      <c r="FT1" s="225"/>
-      <c r="FU1" s="225"/>
-      <c r="FV1" s="225"/>
-      <c r="FW1" s="225"/>
-      <c r="FX1" s="225"/>
-      <c r="FY1" s="225"/>
-      <c r="FZ1" s="225"/>
-      <c r="GA1" s="225"/>
-      <c r="GB1" s="225"/>
-      <c r="GC1" s="225"/>
-      <c r="GD1" s="225"/>
-      <c r="GE1" s="225"/>
-      <c r="GF1" s="225"/>
-      <c r="GG1" s="225"/>
-      <c r="GH1" s="225"/>
-      <c r="GI1" s="225"/>
-      <c r="GJ1" s="225"/>
-      <c r="GK1" s="225"/>
-      <c r="GL1" s="225"/>
-      <c r="GM1" s="225"/>
-      <c r="GN1" s="225"/>
-      <c r="GO1" s="225"/>
-      <c r="GP1" s="225"/>
-      <c r="GQ1" s="225"/>
-      <c r="GR1" s="225"/>
-      <c r="GS1" s="225"/>
-      <c r="GT1" s="225"/>
-      <c r="GU1" s="225"/>
-      <c r="GV1" s="225"/>
-      <c r="GW1" s="225"/>
-      <c r="GX1" s="225"/>
-      <c r="GY1" s="225"/>
-      <c r="GZ1" s="225"/>
-      <c r="HA1" s="225"/>
-      <c r="HB1" s="225"/>
-      <c r="HC1" s="225"/>
-      <c r="HD1" s="225"/>
-      <c r="HE1" s="225"/>
-      <c r="HF1" s="225"/>
-      <c r="HG1" s="225"/>
-      <c r="HH1" s="225"/>
-      <c r="HI1" s="225"/>
-      <c r="HJ1" s="225"/>
-      <c r="HK1" s="225"/>
-      <c r="HL1" s="225"/>
-      <c r="HM1" s="225"/>
-      <c r="HN1" s="225"/>
-      <c r="HO1" s="225"/>
-      <c r="HP1" s="225"/>
-      <c r="HQ1" s="225"/>
-      <c r="HR1" s="225"/>
-      <c r="HS1" s="225"/>
-      <c r="HT1" s="225"/>
-      <c r="HU1" s="225"/>
-      <c r="HV1" s="225"/>
-      <c r="HW1" s="225"/>
-      <c r="HX1" s="225"/>
-      <c r="HY1" s="225"/>
-      <c r="HZ1" s="225"/>
-      <c r="IA1" s="225"/>
-      <c r="IB1" s="225"/>
-      <c r="IC1" s="225"/>
-      <c r="ID1" s="225"/>
-      <c r="IE1" s="225"/>
-      <c r="IF1" s="225"/>
-      <c r="IG1" s="225"/>
-      <c r="IH1" s="225"/>
-      <c r="II1" s="225"/>
-      <c r="IJ1" s="225"/>
-      <c r="IK1" s="225"/>
-      <c r="IL1" s="225"/>
-      <c r="IM1" s="225"/>
-      <c r="IN1" s="225"/>
-      <c r="IO1" s="225"/>
-      <c r="IP1" s="225"/>
-      <c r="IQ1" s="225"/>
-      <c r="IR1" s="225"/>
-      <c r="IS1" s="225"/>
-      <c r="IT1" s="225"/>
-      <c r="IU1" s="225"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+      <c r="H1" s="227"/>
+      <c r="I1" s="227"/>
+      <c r="J1" s="227"/>
+      <c r="K1" s="227"/>
+      <c r="L1" s="227"/>
+      <c r="M1" s="227"/>
+      <c r="N1" s="227"/>
+      <c r="O1" s="227"/>
+      <c r="P1" s="227"/>
+      <c r="Q1" s="227"/>
+      <c r="R1" s="227"/>
+      <c r="S1" s="227"/>
+      <c r="T1" s="227"/>
+      <c r="U1" s="227"/>
+      <c r="V1" s="227"/>
+      <c r="W1" s="227"/>
+      <c r="X1" s="227"/>
+      <c r="Y1" s="227"/>
+      <c r="Z1" s="227"/>
+      <c r="AA1" s="227"/>
+      <c r="AB1" s="227"/>
+      <c r="AC1" s="227"/>
+      <c r="AD1" s="227"/>
+      <c r="AE1" s="227"/>
+      <c r="AF1" s="227"/>
+      <c r="AG1" s="227"/>
+      <c r="AH1" s="227"/>
+      <c r="AI1" s="227"/>
+      <c r="AJ1" s="227"/>
+      <c r="AK1" s="227"/>
+      <c r="AL1" s="227"/>
+      <c r="AM1" s="227"/>
+      <c r="AN1" s="227"/>
+      <c r="AO1" s="227"/>
+      <c r="AP1" s="227"/>
+      <c r="AQ1" s="227"/>
+      <c r="AR1" s="227"/>
+      <c r="AS1" s="227"/>
+      <c r="AT1" s="227"/>
+      <c r="AU1" s="227"/>
+      <c r="AV1" s="227"/>
+      <c r="AW1" s="227"/>
+      <c r="AX1" s="227"/>
+      <c r="AY1" s="227"/>
+      <c r="AZ1" s="227"/>
+      <c r="BA1" s="227"/>
+      <c r="BB1" s="227"/>
+      <c r="BC1" s="227"/>
+      <c r="BD1" s="227"/>
+      <c r="BE1" s="227"/>
+      <c r="BF1" s="227"/>
+      <c r="BG1" s="227"/>
+      <c r="BH1" s="227"/>
+      <c r="BI1" s="227"/>
+      <c r="BJ1" s="227"/>
+      <c r="BK1" s="227"/>
+      <c r="BL1" s="227"/>
+      <c r="BM1" s="227"/>
+      <c r="BN1" s="227"/>
+      <c r="BO1" s="227"/>
+      <c r="BP1" s="227"/>
+      <c r="BQ1" s="227"/>
+      <c r="BR1" s="227"/>
+      <c r="BS1" s="227"/>
+      <c r="BT1" s="227"/>
+      <c r="BU1" s="227"/>
+      <c r="BV1" s="227"/>
+      <c r="BW1" s="227"/>
+      <c r="BX1" s="227"/>
+      <c r="BY1" s="227"/>
+      <c r="BZ1" s="227"/>
+      <c r="CA1" s="227"/>
+      <c r="CB1" s="227"/>
+      <c r="CC1" s="227"/>
+      <c r="CD1" s="227"/>
+      <c r="CE1" s="227"/>
+      <c r="CF1" s="227"/>
+      <c r="CG1" s="227"/>
+      <c r="CH1" s="227"/>
+      <c r="CI1" s="227"/>
+      <c r="CJ1" s="227"/>
+      <c r="CK1" s="227"/>
+      <c r="CL1" s="227"/>
+      <c r="CM1" s="227"/>
+      <c r="CN1" s="227"/>
+      <c r="CO1" s="227"/>
+      <c r="CP1" s="227"/>
+      <c r="CQ1" s="227"/>
+      <c r="CR1" s="227"/>
+      <c r="CS1" s="227"/>
+      <c r="CT1" s="227"/>
+      <c r="CU1" s="227"/>
+      <c r="CV1" s="227"/>
+      <c r="CW1" s="227"/>
+      <c r="CX1" s="227"/>
+      <c r="CY1" s="227"/>
+      <c r="CZ1" s="227"/>
+      <c r="DA1" s="227"/>
+      <c r="DB1" s="227"/>
+      <c r="DC1" s="227"/>
+      <c r="DD1" s="227"/>
+      <c r="DE1" s="227"/>
+      <c r="DF1" s="227"/>
+      <c r="DG1" s="227"/>
+      <c r="DH1" s="227"/>
+      <c r="DI1" s="227"/>
+      <c r="DJ1" s="227"/>
+      <c r="DK1" s="227"/>
+      <c r="DL1" s="227"/>
+      <c r="DM1" s="227"/>
+      <c r="DN1" s="227"/>
+      <c r="DO1" s="227"/>
+      <c r="DP1" s="227"/>
+      <c r="DQ1" s="227"/>
+      <c r="DR1" s="227"/>
+      <c r="DS1" s="227"/>
+      <c r="DT1" s="227"/>
+      <c r="DU1" s="227"/>
+      <c r="DV1" s="227"/>
+      <c r="DW1" s="227"/>
+      <c r="DX1" s="227"/>
+      <c r="DY1" s="227"/>
+      <c r="DZ1" s="227"/>
+      <c r="EA1" s="227"/>
+      <c r="EB1" s="227"/>
+      <c r="EC1" s="227"/>
+      <c r="ED1" s="227"/>
+      <c r="EE1" s="227"/>
+      <c r="EF1" s="227"/>
+      <c r="EG1" s="227"/>
+      <c r="EH1" s="227"/>
+      <c r="EI1" s="227"/>
+      <c r="EJ1" s="227"/>
+      <c r="EK1" s="227"/>
+      <c r="EL1" s="227"/>
+      <c r="EM1" s="227"/>
+      <c r="EN1" s="227"/>
+      <c r="EO1" s="227"/>
+      <c r="EP1" s="227"/>
+      <c r="EQ1" s="227"/>
+      <c r="ER1" s="227"/>
+      <c r="ES1" s="227"/>
+      <c r="ET1" s="227"/>
+      <c r="EU1" s="227"/>
+      <c r="EV1" s="227"/>
+      <c r="EW1" s="227"/>
+      <c r="EX1" s="227"/>
+      <c r="EY1" s="227"/>
+      <c r="EZ1" s="227"/>
+      <c r="FA1" s="227"/>
+      <c r="FB1" s="227"/>
+      <c r="FC1" s="227"/>
+      <c r="FD1" s="227"/>
+      <c r="FE1" s="227"/>
+      <c r="FF1" s="227"/>
+      <c r="FG1" s="227"/>
+      <c r="FH1" s="227"/>
+      <c r="FI1" s="227"/>
+      <c r="FJ1" s="227"/>
+      <c r="FK1" s="227"/>
+      <c r="FL1" s="227"/>
+      <c r="FM1" s="227"/>
+      <c r="FN1" s="227"/>
+      <c r="FO1" s="227"/>
+      <c r="FP1" s="227"/>
+      <c r="FQ1" s="227"/>
+      <c r="FR1" s="227"/>
+      <c r="FS1" s="227"/>
+      <c r="FT1" s="227"/>
+      <c r="FU1" s="227"/>
+      <c r="FV1" s="227"/>
+      <c r="FW1" s="227"/>
+      <c r="FX1" s="227"/>
+      <c r="FY1" s="227"/>
+      <c r="FZ1" s="227"/>
+      <c r="GA1" s="227"/>
+      <c r="GB1" s="227"/>
+      <c r="GC1" s="227"/>
+      <c r="GD1" s="227"/>
+      <c r="GE1" s="227"/>
+      <c r="GF1" s="227"/>
+      <c r="GG1" s="227"/>
+      <c r="GH1" s="227"/>
+      <c r="GI1" s="227"/>
+      <c r="GJ1" s="227"/>
+      <c r="GK1" s="227"/>
+      <c r="GL1" s="227"/>
+      <c r="GM1" s="227"/>
+      <c r="GN1" s="227"/>
+      <c r="GO1" s="227"/>
+      <c r="GP1" s="227"/>
+      <c r="GQ1" s="227"/>
+      <c r="GR1" s="227"/>
+      <c r="GS1" s="227"/>
+      <c r="GT1" s="227"/>
+      <c r="GU1" s="227"/>
+      <c r="GV1" s="227"/>
+      <c r="GW1" s="227"/>
+      <c r="GX1" s="227"/>
+      <c r="GY1" s="227"/>
+      <c r="GZ1" s="227"/>
+      <c r="HA1" s="227"/>
+      <c r="HB1" s="227"/>
+      <c r="HC1" s="227"/>
+      <c r="HD1" s="227"/>
+      <c r="HE1" s="227"/>
+      <c r="HF1" s="227"/>
+      <c r="HG1" s="227"/>
+      <c r="HH1" s="227"/>
+      <c r="HI1" s="227"/>
+      <c r="HJ1" s="227"/>
+      <c r="HK1" s="227"/>
+      <c r="HL1" s="227"/>
+      <c r="HM1" s="227"/>
+      <c r="HN1" s="227"/>
+      <c r="HO1" s="227"/>
+      <c r="HP1" s="227"/>
+      <c r="HQ1" s="227"/>
+      <c r="HR1" s="227"/>
+      <c r="HS1" s="227"/>
+      <c r="HT1" s="227"/>
+      <c r="HU1" s="227"/>
+      <c r="HV1" s="227"/>
+      <c r="HW1" s="227"/>
+      <c r="HX1" s="227"/>
+      <c r="HY1" s="227"/>
+      <c r="HZ1" s="227"/>
+      <c r="IA1" s="227"/>
+      <c r="IB1" s="227"/>
+      <c r="IC1" s="227"/>
+      <c r="ID1" s="227"/>
+      <c r="IE1" s="227"/>
+      <c r="IF1" s="227"/>
+      <c r="IG1" s="227"/>
+      <c r="IH1" s="227"/>
+      <c r="II1" s="227"/>
+      <c r="IJ1" s="227"/>
+      <c r="IK1" s="227"/>
+      <c r="IL1" s="227"/>
+      <c r="IM1" s="227"/>
+      <c r="IN1" s="227"/>
+      <c r="IO1" s="227"/>
+      <c r="IP1" s="227"/>
+      <c r="IQ1" s="227"/>
+      <c r="IR1" s="227"/>
+      <c r="IS1" s="227"/>
+      <c r="IT1" s="227"/>
+      <c r="IU1" s="227"/>
     </row>
     <row r="2" spans="1:255" ht="15.75" thickBot="1">
-      <c r="A2" s="228" t="str">
+      <c r="A2" s="230" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
     </row>
     <row r="3" spans="1:255" ht="15" customHeight="1">
-      <c r="A3" s="229" t="str">
+      <c r="A3" s="231" t="str">
         <f>'Сводная таблица'!A3:A4</f>
         <v>№ п/п</v>
       </c>
-      <c r="B3" s="231" t="str">
+      <c r="B3" s="233" t="str">
         <f>'Сводная таблица'!B3:B4</f>
         <v>группа</v>
       </c>
-      <c r="C3" s="233" t="str">
+      <c r="C3" s="235" t="str">
         <f>'Сводная таблица'!C3:C4</f>
         <v>подргуппа</v>
       </c>
-      <c r="D3" s="235" t="str">
+      <c r="D3" s="237" t="str">
         <f>'Сводная таблица'!D3:D4</f>
         <v>Фамилия</v>
       </c>
-      <c r="E3" s="237" t="str">
+      <c r="E3" s="239" t="str">
         <f>'Сводная таблица'!E3:E4</f>
         <v>Имя</v>
       </c>
-      <c r="F3" s="226" t="str">
+      <c r="F3" s="228" t="str">
         <f>'Сводная таблица'!F3:F4</f>
         <v>Отчество</v>
       </c>
-      <c r="G3" s="229" t="s">
+      <c r="G3" s="231" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="235" t="s">
+      <c r="H3" s="237" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="242" t="s">
+      <c r="I3" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="242" t="s">
+      <c r="J3" s="244" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="239" t="s">
+      <c r="K3" s="241" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="249" t="s">
+      <c r="L3" s="251" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:255" ht="15.75" thickBot="1">
-      <c r="A4" s="230"/>
-      <c r="B4" s="232"/>
-      <c r="C4" s="234"/>
-      <c r="D4" s="236"/>
-      <c r="E4" s="238"/>
-      <c r="F4" s="227"/>
-      <c r="G4" s="230"/>
-      <c r="H4" s="236"/>
-      <c r="I4" s="246"/>
-      <c r="J4" s="246"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="250"/>
+      <c r="A4" s="232"/>
+      <c r="B4" s="234"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="238"/>
+      <c r="E4" s="240"/>
+      <c r="F4" s="229"/>
+      <c r="G4" s="232"/>
+      <c r="H4" s="238"/>
+      <c r="I4" s="248"/>
+      <c r="J4" s="248"/>
+      <c r="K4" s="253"/>
+      <c r="L4" s="252"/>
     </row>
     <row r="5" spans="1:255" s="40" customFormat="1">
       <c r="A5" s="145">
@@ -54646,338 +54645,338 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="227" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
-      <c r="G1" s="225"/>
-      <c r="H1" s="225"/>
-      <c r="I1" s="225"/>
-      <c r="J1" s="225"/>
-      <c r="K1" s="225"/>
-      <c r="L1" s="225"/>
-      <c r="M1" s="225"/>
-      <c r="N1" s="225"/>
-      <c r="O1" s="225"/>
-      <c r="P1" s="225"/>
-      <c r="Q1" s="225"/>
-      <c r="R1" s="225"/>
-      <c r="S1" s="225"/>
-      <c r="T1" s="225"/>
-      <c r="U1" s="225"/>
-      <c r="V1" s="225"/>
-      <c r="W1" s="225"/>
-      <c r="X1" s="225"/>
-      <c r="Y1" s="225"/>
-      <c r="Z1" s="225"/>
-      <c r="AA1" s="225"/>
-      <c r="AB1" s="225"/>
-      <c r="AC1" s="225"/>
-      <c r="AD1" s="225"/>
-      <c r="AE1" s="225"/>
-      <c r="AF1" s="225"/>
-      <c r="AG1" s="225"/>
-      <c r="AH1" s="225"/>
-      <c r="AI1" s="225"/>
-      <c r="AJ1" s="225"/>
-      <c r="AK1" s="225"/>
-      <c r="AL1" s="225"/>
-      <c r="AM1" s="225"/>
-      <c r="AN1" s="225"/>
-      <c r="AO1" s="225"/>
-      <c r="AP1" s="225"/>
-      <c r="AQ1" s="225"/>
-      <c r="AR1" s="225"/>
-      <c r="AS1" s="225"/>
-      <c r="AT1" s="225"/>
-      <c r="AU1" s="225"/>
-      <c r="AV1" s="225"/>
-      <c r="AW1" s="225"/>
-      <c r="AX1" s="225"/>
-      <c r="AY1" s="225"/>
-      <c r="AZ1" s="225"/>
-      <c r="BA1" s="225"/>
-      <c r="BB1" s="225"/>
-      <c r="BC1" s="225"/>
-      <c r="BD1" s="225"/>
-      <c r="BE1" s="225"/>
-      <c r="BF1" s="225"/>
-      <c r="BG1" s="225"/>
-      <c r="BH1" s="225"/>
-      <c r="BI1" s="225"/>
-      <c r="BJ1" s="225"/>
-      <c r="BK1" s="225"/>
-      <c r="BL1" s="225"/>
-      <c r="BM1" s="225"/>
-      <c r="BN1" s="225"/>
-      <c r="BO1" s="225"/>
-      <c r="BP1" s="225"/>
-      <c r="BQ1" s="225"/>
-      <c r="BR1" s="225"/>
-      <c r="BS1" s="225"/>
-      <c r="BT1" s="225"/>
-      <c r="BU1" s="225"/>
-      <c r="BV1" s="225"/>
-      <c r="BW1" s="225"/>
-      <c r="BX1" s="225"/>
-      <c r="BY1" s="225"/>
-      <c r="BZ1" s="225"/>
-      <c r="CA1" s="225"/>
-      <c r="CB1" s="225"/>
-      <c r="CC1" s="225"/>
-      <c r="CD1" s="225"/>
-      <c r="CE1" s="225"/>
-      <c r="CF1" s="225"/>
-      <c r="CG1" s="225"/>
-      <c r="CH1" s="225"/>
-      <c r="CI1" s="225"/>
-      <c r="CJ1" s="225"/>
-      <c r="CK1" s="225"/>
-      <c r="CL1" s="225"/>
-      <c r="CM1" s="225"/>
-      <c r="CN1" s="225"/>
-      <c r="CO1" s="225"/>
-      <c r="CP1" s="225"/>
-      <c r="CQ1" s="225"/>
-      <c r="CR1" s="225"/>
-      <c r="CS1" s="225"/>
-      <c r="CT1" s="225"/>
-      <c r="CU1" s="225"/>
-      <c r="CV1" s="225"/>
-      <c r="CW1" s="225"/>
-      <c r="CX1" s="225"/>
-      <c r="CY1" s="225"/>
-      <c r="CZ1" s="225"/>
-      <c r="DA1" s="225"/>
-      <c r="DB1" s="225"/>
-      <c r="DC1" s="225"/>
-      <c r="DD1" s="225"/>
-      <c r="DE1" s="225"/>
-      <c r="DF1" s="225"/>
-      <c r="DG1" s="225"/>
-      <c r="DH1" s="225"/>
-      <c r="DI1" s="225"/>
-      <c r="DJ1" s="225"/>
-      <c r="DK1" s="225"/>
-      <c r="DL1" s="225"/>
-      <c r="DM1" s="225"/>
-      <c r="DN1" s="225"/>
-      <c r="DO1" s="225"/>
-      <c r="DP1" s="225"/>
-      <c r="DQ1" s="225"/>
-      <c r="DR1" s="225"/>
-      <c r="DS1" s="225"/>
-      <c r="DT1" s="225"/>
-      <c r="DU1" s="225"/>
-      <c r="DV1" s="225"/>
-      <c r="DW1" s="225"/>
-      <c r="DX1" s="225"/>
-      <c r="DY1" s="225"/>
-      <c r="DZ1" s="225"/>
-      <c r="EA1" s="225"/>
-      <c r="EB1" s="225"/>
-      <c r="EC1" s="225"/>
-      <c r="ED1" s="225"/>
-      <c r="EE1" s="225"/>
-      <c r="EF1" s="225"/>
-      <c r="EG1" s="225"/>
-      <c r="EH1" s="225"/>
-      <c r="EI1" s="225"/>
-      <c r="EJ1" s="225"/>
-      <c r="EK1" s="225"/>
-      <c r="EL1" s="225"/>
-      <c r="EM1" s="225"/>
-      <c r="EN1" s="225"/>
-      <c r="EO1" s="225"/>
-      <c r="EP1" s="225"/>
-      <c r="EQ1" s="225"/>
-      <c r="ER1" s="225"/>
-      <c r="ES1" s="225"/>
-      <c r="ET1" s="225"/>
-      <c r="EU1" s="225"/>
-      <c r="EV1" s="225"/>
-      <c r="EW1" s="225"/>
-      <c r="EX1" s="225"/>
-      <c r="EY1" s="225"/>
-      <c r="EZ1" s="225"/>
-      <c r="FA1" s="225"/>
-      <c r="FB1" s="225"/>
-      <c r="FC1" s="225"/>
-      <c r="FD1" s="225"/>
-      <c r="FE1" s="225"/>
-      <c r="FF1" s="225"/>
-      <c r="FG1" s="225"/>
-      <c r="FH1" s="225"/>
-      <c r="FI1" s="225"/>
-      <c r="FJ1" s="225"/>
-      <c r="FK1" s="225"/>
-      <c r="FL1" s="225"/>
-      <c r="FM1" s="225"/>
-      <c r="FN1" s="225"/>
-      <c r="FO1" s="225"/>
-      <c r="FP1" s="225"/>
-      <c r="FQ1" s="225"/>
-      <c r="FR1" s="225"/>
-      <c r="FS1" s="225"/>
-      <c r="FT1" s="225"/>
-      <c r="FU1" s="225"/>
-      <c r="FV1" s="225"/>
-      <c r="FW1" s="225"/>
-      <c r="FX1" s="225"/>
-      <c r="FY1" s="225"/>
-      <c r="FZ1" s="225"/>
-      <c r="GA1" s="225"/>
-      <c r="GB1" s="225"/>
-      <c r="GC1" s="225"/>
-      <c r="GD1" s="225"/>
-      <c r="GE1" s="225"/>
-      <c r="GF1" s="225"/>
-      <c r="GG1" s="225"/>
-      <c r="GH1" s="225"/>
-      <c r="GI1" s="225"/>
-      <c r="GJ1" s="225"/>
-      <c r="GK1" s="225"/>
-      <c r="GL1" s="225"/>
-      <c r="GM1" s="225"/>
-      <c r="GN1" s="225"/>
-      <c r="GO1" s="225"/>
-      <c r="GP1" s="225"/>
-      <c r="GQ1" s="225"/>
-      <c r="GR1" s="225"/>
-      <c r="GS1" s="225"/>
-      <c r="GT1" s="225"/>
-      <c r="GU1" s="225"/>
-      <c r="GV1" s="225"/>
-      <c r="GW1" s="225"/>
-      <c r="GX1" s="225"/>
-      <c r="GY1" s="225"/>
-      <c r="GZ1" s="225"/>
-      <c r="HA1" s="225"/>
-      <c r="HB1" s="225"/>
-      <c r="HC1" s="225"/>
-      <c r="HD1" s="225"/>
-      <c r="HE1" s="225"/>
-      <c r="HF1" s="225"/>
-      <c r="HG1" s="225"/>
-      <c r="HH1" s="225"/>
-      <c r="HI1" s="225"/>
-      <c r="HJ1" s="225"/>
-      <c r="HK1" s="225"/>
-      <c r="HL1" s="225"/>
-      <c r="HM1" s="225"/>
-      <c r="HN1" s="225"/>
-      <c r="HO1" s="225"/>
-      <c r="HP1" s="225"/>
-      <c r="HQ1" s="225"/>
-      <c r="HR1" s="225"/>
-      <c r="HS1" s="225"/>
-      <c r="HT1" s="225"/>
-      <c r="HU1" s="225"/>
-      <c r="HV1" s="225"/>
-      <c r="HW1" s="225"/>
-      <c r="HX1" s="225"/>
-      <c r="HY1" s="225"/>
-      <c r="HZ1" s="225"/>
-      <c r="IA1" s="225"/>
-      <c r="IB1" s="225"/>
-      <c r="IC1" s="225"/>
-      <c r="ID1" s="225"/>
-      <c r="IE1" s="225"/>
-      <c r="IF1" s="225"/>
-      <c r="IG1" s="225"/>
-      <c r="IH1" s="225"/>
-      <c r="II1" s="225"/>
-      <c r="IJ1" s="225"/>
-      <c r="IK1" s="225"/>
-      <c r="IL1" s="225"/>
-      <c r="IM1" s="225"/>
-      <c r="IN1" s="225"/>
-      <c r="IO1" s="225"/>
-      <c r="IP1" s="225"/>
-      <c r="IQ1" s="225"/>
-      <c r="IR1" s="225"/>
-      <c r="IS1" s="225"/>
-      <c r="IT1" s="225"/>
-      <c r="IU1" s="225"/>
-      <c r="IV1" s="225"/>
+      <c r="B1" s="227"/>
+      <c r="C1" s="227"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+      <c r="H1" s="227"/>
+      <c r="I1" s="227"/>
+      <c r="J1" s="227"/>
+      <c r="K1" s="227"/>
+      <c r="L1" s="227"/>
+      <c r="M1" s="227"/>
+      <c r="N1" s="227"/>
+      <c r="O1" s="227"/>
+      <c r="P1" s="227"/>
+      <c r="Q1" s="227"/>
+      <c r="R1" s="227"/>
+      <c r="S1" s="227"/>
+      <c r="T1" s="227"/>
+      <c r="U1" s="227"/>
+      <c r="V1" s="227"/>
+      <c r="W1" s="227"/>
+      <c r="X1" s="227"/>
+      <c r="Y1" s="227"/>
+      <c r="Z1" s="227"/>
+      <c r="AA1" s="227"/>
+      <c r="AB1" s="227"/>
+      <c r="AC1" s="227"/>
+      <c r="AD1" s="227"/>
+      <c r="AE1" s="227"/>
+      <c r="AF1" s="227"/>
+      <c r="AG1" s="227"/>
+      <c r="AH1" s="227"/>
+      <c r="AI1" s="227"/>
+      <c r="AJ1" s="227"/>
+      <c r="AK1" s="227"/>
+      <c r="AL1" s="227"/>
+      <c r="AM1" s="227"/>
+      <c r="AN1" s="227"/>
+      <c r="AO1" s="227"/>
+      <c r="AP1" s="227"/>
+      <c r="AQ1" s="227"/>
+      <c r="AR1" s="227"/>
+      <c r="AS1" s="227"/>
+      <c r="AT1" s="227"/>
+      <c r="AU1" s="227"/>
+      <c r="AV1" s="227"/>
+      <c r="AW1" s="227"/>
+      <c r="AX1" s="227"/>
+      <c r="AY1" s="227"/>
+      <c r="AZ1" s="227"/>
+      <c r="BA1" s="227"/>
+      <c r="BB1" s="227"/>
+      <c r="BC1" s="227"/>
+      <c r="BD1" s="227"/>
+      <c r="BE1" s="227"/>
+      <c r="BF1" s="227"/>
+      <c r="BG1" s="227"/>
+      <c r="BH1" s="227"/>
+      <c r="BI1" s="227"/>
+      <c r="BJ1" s="227"/>
+      <c r="BK1" s="227"/>
+      <c r="BL1" s="227"/>
+      <c r="BM1" s="227"/>
+      <c r="BN1" s="227"/>
+      <c r="BO1" s="227"/>
+      <c r="BP1" s="227"/>
+      <c r="BQ1" s="227"/>
+      <c r="BR1" s="227"/>
+      <c r="BS1" s="227"/>
+      <c r="BT1" s="227"/>
+      <c r="BU1" s="227"/>
+      <c r="BV1" s="227"/>
+      <c r="BW1" s="227"/>
+      <c r="BX1" s="227"/>
+      <c r="BY1" s="227"/>
+      <c r="BZ1" s="227"/>
+      <c r="CA1" s="227"/>
+      <c r="CB1" s="227"/>
+      <c r="CC1" s="227"/>
+      <c r="CD1" s="227"/>
+      <c r="CE1" s="227"/>
+      <c r="CF1" s="227"/>
+      <c r="CG1" s="227"/>
+      <c r="CH1" s="227"/>
+      <c r="CI1" s="227"/>
+      <c r="CJ1" s="227"/>
+      <c r="CK1" s="227"/>
+      <c r="CL1" s="227"/>
+      <c r="CM1" s="227"/>
+      <c r="CN1" s="227"/>
+      <c r="CO1" s="227"/>
+      <c r="CP1" s="227"/>
+      <c r="CQ1" s="227"/>
+      <c r="CR1" s="227"/>
+      <c r="CS1" s="227"/>
+      <c r="CT1" s="227"/>
+      <c r="CU1" s="227"/>
+      <c r="CV1" s="227"/>
+      <c r="CW1" s="227"/>
+      <c r="CX1" s="227"/>
+      <c r="CY1" s="227"/>
+      <c r="CZ1" s="227"/>
+      <c r="DA1" s="227"/>
+      <c r="DB1" s="227"/>
+      <c r="DC1" s="227"/>
+      <c r="DD1" s="227"/>
+      <c r="DE1" s="227"/>
+      <c r="DF1" s="227"/>
+      <c r="DG1" s="227"/>
+      <c r="DH1" s="227"/>
+      <c r="DI1" s="227"/>
+      <c r="DJ1" s="227"/>
+      <c r="DK1" s="227"/>
+      <c r="DL1" s="227"/>
+      <c r="DM1" s="227"/>
+      <c r="DN1" s="227"/>
+      <c r="DO1" s="227"/>
+      <c r="DP1" s="227"/>
+      <c r="DQ1" s="227"/>
+      <c r="DR1" s="227"/>
+      <c r="DS1" s="227"/>
+      <c r="DT1" s="227"/>
+      <c r="DU1" s="227"/>
+      <c r="DV1" s="227"/>
+      <c r="DW1" s="227"/>
+      <c r="DX1" s="227"/>
+      <c r="DY1" s="227"/>
+      <c r="DZ1" s="227"/>
+      <c r="EA1" s="227"/>
+      <c r="EB1" s="227"/>
+      <c r="EC1" s="227"/>
+      <c r="ED1" s="227"/>
+      <c r="EE1" s="227"/>
+      <c r="EF1" s="227"/>
+      <c r="EG1" s="227"/>
+      <c r="EH1" s="227"/>
+      <c r="EI1" s="227"/>
+      <c r="EJ1" s="227"/>
+      <c r="EK1" s="227"/>
+      <c r="EL1" s="227"/>
+      <c r="EM1" s="227"/>
+      <c r="EN1" s="227"/>
+      <c r="EO1" s="227"/>
+      <c r="EP1" s="227"/>
+      <c r="EQ1" s="227"/>
+      <c r="ER1" s="227"/>
+      <c r="ES1" s="227"/>
+      <c r="ET1" s="227"/>
+      <c r="EU1" s="227"/>
+      <c r="EV1" s="227"/>
+      <c r="EW1" s="227"/>
+      <c r="EX1" s="227"/>
+      <c r="EY1" s="227"/>
+      <c r="EZ1" s="227"/>
+      <c r="FA1" s="227"/>
+      <c r="FB1" s="227"/>
+      <c r="FC1" s="227"/>
+      <c r="FD1" s="227"/>
+      <c r="FE1" s="227"/>
+      <c r="FF1" s="227"/>
+      <c r="FG1" s="227"/>
+      <c r="FH1" s="227"/>
+      <c r="FI1" s="227"/>
+      <c r="FJ1" s="227"/>
+      <c r="FK1" s="227"/>
+      <c r="FL1" s="227"/>
+      <c r="FM1" s="227"/>
+      <c r="FN1" s="227"/>
+      <c r="FO1" s="227"/>
+      <c r="FP1" s="227"/>
+      <c r="FQ1" s="227"/>
+      <c r="FR1" s="227"/>
+      <c r="FS1" s="227"/>
+      <c r="FT1" s="227"/>
+      <c r="FU1" s="227"/>
+      <c r="FV1" s="227"/>
+      <c r="FW1" s="227"/>
+      <c r="FX1" s="227"/>
+      <c r="FY1" s="227"/>
+      <c r="FZ1" s="227"/>
+      <c r="GA1" s="227"/>
+      <c r="GB1" s="227"/>
+      <c r="GC1" s="227"/>
+      <c r="GD1" s="227"/>
+      <c r="GE1" s="227"/>
+      <c r="GF1" s="227"/>
+      <c r="GG1" s="227"/>
+      <c r="GH1" s="227"/>
+      <c r="GI1" s="227"/>
+      <c r="GJ1" s="227"/>
+      <c r="GK1" s="227"/>
+      <c r="GL1" s="227"/>
+      <c r="GM1" s="227"/>
+      <c r="GN1" s="227"/>
+      <c r="GO1" s="227"/>
+      <c r="GP1" s="227"/>
+      <c r="GQ1" s="227"/>
+      <c r="GR1" s="227"/>
+      <c r="GS1" s="227"/>
+      <c r="GT1" s="227"/>
+      <c r="GU1" s="227"/>
+      <c r="GV1" s="227"/>
+      <c r="GW1" s="227"/>
+      <c r="GX1" s="227"/>
+      <c r="GY1" s="227"/>
+      <c r="GZ1" s="227"/>
+      <c r="HA1" s="227"/>
+      <c r="HB1" s="227"/>
+      <c r="HC1" s="227"/>
+      <c r="HD1" s="227"/>
+      <c r="HE1" s="227"/>
+      <c r="HF1" s="227"/>
+      <c r="HG1" s="227"/>
+      <c r="HH1" s="227"/>
+      <c r="HI1" s="227"/>
+      <c r="HJ1" s="227"/>
+      <c r="HK1" s="227"/>
+      <c r="HL1" s="227"/>
+      <c r="HM1" s="227"/>
+      <c r="HN1" s="227"/>
+      <c r="HO1" s="227"/>
+      <c r="HP1" s="227"/>
+      <c r="HQ1" s="227"/>
+      <c r="HR1" s="227"/>
+      <c r="HS1" s="227"/>
+      <c r="HT1" s="227"/>
+      <c r="HU1" s="227"/>
+      <c r="HV1" s="227"/>
+      <c r="HW1" s="227"/>
+      <c r="HX1" s="227"/>
+      <c r="HY1" s="227"/>
+      <c r="HZ1" s="227"/>
+      <c r="IA1" s="227"/>
+      <c r="IB1" s="227"/>
+      <c r="IC1" s="227"/>
+      <c r="ID1" s="227"/>
+      <c r="IE1" s="227"/>
+      <c r="IF1" s="227"/>
+      <c r="IG1" s="227"/>
+      <c r="IH1" s="227"/>
+      <c r="II1" s="227"/>
+      <c r="IJ1" s="227"/>
+      <c r="IK1" s="227"/>
+      <c r="IL1" s="227"/>
+      <c r="IM1" s="227"/>
+      <c r="IN1" s="227"/>
+      <c r="IO1" s="227"/>
+      <c r="IP1" s="227"/>
+      <c r="IQ1" s="227"/>
+      <c r="IR1" s="227"/>
+      <c r="IS1" s="227"/>
+      <c r="IT1" s="227"/>
+      <c r="IU1" s="227"/>
+      <c r="IV1" s="227"/>
     </row>
     <row r="2" spans="1:256" ht="15.75" thickBot="1">
-      <c r="A2" s="228" t="str">
+      <c r="A2" s="230" t="str">
         <f>'Сводная таблица'!D2</f>
         <v>Группы 114 05 115 - 114 05 215</v>
       </c>
-      <c r="B2" s="228"/>
-      <c r="C2" s="228"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="228"/>
-      <c r="F2" s="228"/>
-      <c r="G2" s="228"/>
-      <c r="H2" s="228"/>
-      <c r="I2" s="228"/>
-      <c r="J2" s="228"/>
-      <c r="K2" s="228"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
+      <c r="E2" s="230"/>
+      <c r="F2" s="230"/>
+      <c r="G2" s="230"/>
+      <c r="H2" s="230"/>
+      <c r="I2" s="230"/>
+      <c r="J2" s="230"/>
+      <c r="K2" s="230"/>
     </row>
     <row r="3" spans="1:256" ht="15" customHeight="1">
-      <c r="A3" s="229" t="str">
+      <c r="A3" s="231" t="str">
         <f>'Сводная таблица'!A3:A4</f>
         <v>№ п/п</v>
       </c>
-      <c r="B3" s="231" t="str">
+      <c r="B3" s="233" t="str">
         <f>'Сводная таблица'!B3:B4</f>
         <v>группа</v>
       </c>
-      <c r="C3" s="233" t="str">
+      <c r="C3" s="235" t="str">
         <f>'Сводная таблица'!C3:C4</f>
         <v>подргуппа</v>
       </c>
-      <c r="D3" s="235" t="str">
+      <c r="D3" s="237" t="str">
         <f>'Сводная таблица'!D3:D4</f>
         <v>Фамилия</v>
       </c>
-      <c r="E3" s="237" t="str">
+      <c r="E3" s="239" t="str">
         <f>'Сводная таблица'!E3:E4</f>
         <v>Имя</v>
       </c>
-      <c r="F3" s="226" t="str">
+      <c r="F3" s="228" t="str">
         <f>'Сводная таблица'!F3:F4</f>
         <v>Отчество</v>
       </c>
-      <c r="G3" s="229" t="s">
+      <c r="G3" s="231" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="235" t="s">
+      <c r="H3" s="237" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="242" t="s">
+      <c r="I3" s="244" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="242" t="s">
+      <c r="J3" s="244" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="247" t="s">
+      <c r="K3" s="249" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="249" t="s">
+      <c r="L3" s="251" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:256" ht="15.75" thickBot="1">
-      <c r="A4" s="230"/>
-      <c r="B4" s="232"/>
-      <c r="C4" s="234"/>
-      <c r="D4" s="236"/>
-      <c r="E4" s="238"/>
-      <c r="F4" s="227"/>
-      <c r="G4" s="230"/>
-      <c r="H4" s="236"/>
-      <c r="I4" s="246"/>
-      <c r="J4" s="246"/>
-      <c r="K4" s="248"/>
-      <c r="L4" s="250"/>
+      <c r="A4" s="232"/>
+      <c r="B4" s="234"/>
+      <c r="C4" s="236"/>
+      <c r="D4" s="238"/>
+      <c r="E4" s="240"/>
+      <c r="F4" s="229"/>
+      <c r="G4" s="232"/>
+      <c r="H4" s="238"/>
+      <c r="I4" s="248"/>
+      <c r="J4" s="248"/>
+      <c r="K4" s="250"/>
+      <c r="L4" s="252"/>
     </row>
     <row r="5" spans="1:256" s="40" customFormat="1" ht="15.75" thickBot="1">
       <c r="A5" s="145">
@@ -56644,8 +56643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB185"/>
   <sheetViews>
-    <sheetView topLeftCell="F73" workbookViewId="0">
-      <selection activeCell="L79" sqref="L79"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -59102,10 +59101,10 @@
       <c r="C71" s="201">
         <v>7.57</v>
       </c>
-      <c r="D71" s="252" t="s">
+      <c r="D71" s="254" t="s">
         <v>201</v>
       </c>
-      <c r="E71" s="252"/>
+      <c r="E71" s="254"/>
       <c r="F71" s="197">
         <v>0.66</v>
       </c>
@@ -59565,47 +59564,47 @@
       <c r="E86" s="169" t="s">
         <v>154</v>
       </c>
-      <c r="F86" s="253">
-        <v>150.37730349012114</v>
+      <c r="F86" s="209">
+        <v>44.330828144757234</v>
       </c>
       <c r="G86" s="171"/>
-      <c r="H86" s="254" t="s">
+      <c r="H86" s="208" t="s">
         <v>171</v>
       </c>
-      <c r="I86" s="255">
+      <c r="I86" s="209">
         <v>144.28</v>
       </c>
-      <c r="J86" s="254" t="s">
+      <c r="J86" s="208" t="s">
         <v>232</v>
       </c>
-      <c r="K86" s="255">
+      <c r="K86" s="209">
         <v>353.22</v>
       </c>
-      <c r="L86" s="254" t="s">
+      <c r="L86" s="208" t="s">
         <v>172</v>
       </c>
-      <c r="M86" s="255">
+      <c r="M86" s="209">
         <v>0.12</v>
       </c>
-      <c r="N86" s="254" t="s">
+      <c r="N86" s="208" t="s">
         <v>191</v>
       </c>
-      <c r="O86" s="255">
+      <c r="O86" s="209">
         <v>0.09</v>
       </c>
-      <c r="P86" s="254" t="s">
+      <c r="P86" s="208" t="s">
         <v>153</v>
       </c>
-      <c r="Q86" s="255">
+      <c r="Q86" s="209">
         <f>I86*K86</f>
         <v>50962.581600000005</v>
       </c>
-      <c r="R86" s="254" t="s">
+      <c r="R86" s="208" t="s">
         <v>154</v>
       </c>
-      <c r="S86" s="255">
-        <f>SQRT(K86*K86*M86*M86+I86*I86+O86*O86)</f>
-        <v>150.37730349012114</v>
+      <c r="S86" s="209">
+        <f>SQRT(K86*K86*M86*M86+I86*I86*O86*O86)</f>
+        <v>44.330828144757234</v>
       </c>
       <c r="T86" s="195"/>
       <c r="U86" s="195"/>
@@ -61295,7 +61294,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection password="961B" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="D71:E71"/>
   </mergeCells>
@@ -61308,8 +61307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -61327,7 +61326,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C21" ca="1" si="0">RAND()</f>
-        <v>0.56832071802876527</v>
+        <v>0.95899311022507927</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -61339,7 +61338,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22264697772555841</v>
+        <v>0.9832037336918944</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -61351,7 +61350,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77079178155501826</v>
+        <v>0.45403064654531544</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -61363,7 +61362,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26941438902148462</v>
+        <v>0.88111550250062898</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -61375,7 +61374,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16415742875159012</v>
+        <v>0.20483313323049313</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -61387,7 +61386,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71249281395517716</v>
+        <v>0.45588258116606362</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -61399,7 +61398,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43557493983524598</v>
+        <v>0.84783165078198053</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -61411,7 +61410,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18974987725314474</v>
+        <v>0.50859822103155694</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -61423,7 +61422,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22076131300357194</v>
+        <v>0.88738973460883397</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -61435,7 +61434,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74401148875353051</v>
+        <v>6.084509498719104E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -61447,7 +61446,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39853570990414727</v>
+        <v>0.63736879507772048</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -61459,7 +61458,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65598544958437532</v>
+        <v>0.51102482794132809</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -61471,7 +61470,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56745891783292812</v>
+        <v>0.18078934930478585</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -61483,7 +61482,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83945551434880983</v>
+        <v>0.88283984004083216</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -61495,7 +61494,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30817539404422334</v>
+        <v>0.72681724656363311</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -61507,7 +61506,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55220968201915288</v>
+        <v>0.12191915283284249</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -61519,7 +61518,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85164255502035591</v>
+        <v>0.78721369963222898</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -61531,7 +61530,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88610784711260759</v>
+        <v>0.35984527239751252</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -61543,7 +61542,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92581554282904244</v>
+        <v>0.98348299927724803</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1">
@@ -61555,7 +61554,7 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63007375215566785</v>
+        <v>0.63674143352430357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>